<commit_message>
commit ui with new wiring connecting (#1090)
Co-authored-by: 汤永靖 <tangyongjing@thape.com.cn>
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/连线功能白名单.xlsx
+++ b/AutoLoader/Contents/Support/连线功能白名单.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="324">
   <si>
     <t>名称</t>
   </si>
@@ -527,44 +527,6 @@
     <t>回路2</t>
   </si>
   <si>
-    <t>E-EFPS-WIRE</t>
-  </si>
-  <si>
-    <t>E-FAS-WIRE</t>
-  </si>
-  <si>
-    <t>E-CTRL-WIRE</t>
-  </si>
-  <si>
-    <t>E-FDS-WIRE</t>
-  </si>
-  <si>
-    <t>E-FAS-WIRE5</t>
-  </si>
-  <si>
-    <t>E-FAS-WIRE5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-PMFE-WIRE</t>
-  </si>
-  <si>
-    <t>E-FAS-WIRE2</t>
-  </si>
-  <si>
-    <t>E-BRST-WIRE</t>
-  </si>
-  <si>
-    <t>E-FAS-WIRE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-FAS-WIRE4</t>
-  </si>
-  <si>
-    <t>E-FAS-WIRE3</t>
-  </si>
-  <si>
     <t>起点块：E-BFAS010</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -602,10 +564,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>E-LITE-WIRE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>简式荧光灯（壁装）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -967,13 +925,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>E-LITE-WIRE2</t>
-  </si>
-  <si>
-    <t>E-LITE-WIRE2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>E-BFEL161</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1120,6 +1071,42 @@
   <si>
     <t>消防应急疏散照明灯</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>火灾报警总线</t>
+  </si>
+  <si>
+    <t>总线+DC24V电源线</t>
+  </si>
+  <si>
+    <t>可燃气体探测系统布线</t>
+  </si>
+  <si>
+    <t>手动控制线</t>
+  </si>
+  <si>
+    <t>消防电话总线</t>
+  </si>
+  <si>
+    <t>消防联动控制线</t>
+  </si>
+  <si>
+    <t>消防广播线</t>
+  </si>
+  <si>
+    <t>防火门监控系统布线</t>
+  </si>
+  <si>
+    <t>消防电源监控系统布线</t>
+  </si>
+  <si>
+    <t>电气火灾监控系统布线</t>
+  </si>
+  <si>
+    <t>消防应急照明布线</t>
+  </si>
+  <si>
+    <t>平时照明布线</t>
   </si>
 </sst>
 </file>
@@ -1450,20 +1437,20 @@
   <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.75" customWidth="1"/>
+    <col min="4" max="4" width="21.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1491,7 +1478,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>179</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1502,7 +1489,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>179</v>
+        <v>314</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1513,7 +1500,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>179</v>
+        <v>314</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1524,7 +1511,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>179</v>
+        <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1535,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>179</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1546,7 +1533,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>168</v>
+        <v>321</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1557,7 +1544,7 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>168</v>
+        <v>321</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1568,7 +1555,7 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>168</v>
+        <v>321</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1579,7 +1566,7 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>168</v>
+        <v>321</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1590,7 +1577,7 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>168</v>
+        <v>321</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1601,7 +1588,7 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>168</v>
+        <v>321</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1612,7 +1599,7 @@
         <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>168</v>
+        <v>321</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1623,7 +1610,7 @@
         <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>168</v>
+        <v>321</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1634,7 +1621,7 @@
         <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>168</v>
+        <v>321</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1645,7 +1632,7 @@
         <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>168</v>
+        <v>321</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1656,7 +1643,7 @@
         <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>168</v>
+        <v>321</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1667,7 +1654,7 @@
         <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>168</v>
+        <v>321</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1678,10 +1665,10 @@
         <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
       <c r="D20" t="s">
-        <v>175</v>
+        <v>313</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1692,7 +1679,7 @@
         <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1703,7 +1690,7 @@
         <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1714,7 +1701,7 @@
         <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1725,7 +1712,7 @@
         <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1736,7 +1723,7 @@
         <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1747,7 +1734,7 @@
         <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1758,10 +1745,10 @@
         <v>50</v>
       </c>
       <c r="C27" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
       <c r="D27" t="s">
-        <v>175</v>
+        <v>313</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1772,7 +1759,7 @@
         <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1783,7 +1770,7 @@
         <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1794,7 +1781,7 @@
         <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1805,7 +1792,7 @@
         <v>58</v>
       </c>
       <c r="C31" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1816,7 +1803,7 @@
         <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1827,7 +1814,7 @@
         <v>62</v>
       </c>
       <c r="C33" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1838,7 +1825,7 @@
         <v>64</v>
       </c>
       <c r="C34" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1849,7 +1836,7 @@
         <v>66</v>
       </c>
       <c r="C35" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1860,7 +1847,7 @@
         <v>68</v>
       </c>
       <c r="C36" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1871,7 +1858,7 @@
         <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1882,7 +1869,7 @@
         <v>72</v>
       </c>
       <c r="C38" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1893,7 +1880,7 @@
         <v>74</v>
       </c>
       <c r="C39" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1904,7 +1891,7 @@
         <v>76</v>
       </c>
       <c r="C40" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1915,10 +1902,10 @@
         <v>78</v>
       </c>
       <c r="C41" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
       <c r="D41" t="s">
-        <v>175</v>
+        <v>313</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1929,7 +1916,7 @@
         <v>80</v>
       </c>
       <c r="C42" t="s">
-        <v>173</v>
+        <v>316</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1940,7 +1927,7 @@
         <v>82</v>
       </c>
       <c r="C43" t="s">
-        <v>172</v>
+        <v>316</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1951,7 +1938,7 @@
         <v>84</v>
       </c>
       <c r="C44" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1962,7 +1949,7 @@
         <v>86</v>
       </c>
       <c r="C45" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1973,7 +1960,7 @@
         <v>88</v>
       </c>
       <c r="C46" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1984,7 +1971,7 @@
         <v>90</v>
       </c>
       <c r="C47" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1995,7 +1982,7 @@
         <v>92</v>
       </c>
       <c r="C48" t="s">
-        <v>176</v>
+        <v>318</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -2006,7 +1993,7 @@
         <v>92</v>
       </c>
       <c r="C49" t="s">
-        <v>176</v>
+        <v>318</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -2017,7 +2004,7 @@
         <v>92</v>
       </c>
       <c r="C50" t="s">
-        <v>176</v>
+        <v>318</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -2028,7 +2015,7 @@
         <v>96</v>
       </c>
       <c r="C51" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -2039,7 +2026,7 @@
         <v>98</v>
       </c>
       <c r="C52" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -2050,10 +2037,10 @@
         <v>100</v>
       </c>
       <c r="C53" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
       <c r="D53" t="s">
-        <v>175</v>
+        <v>313</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -2064,10 +2051,10 @@
         <v>102</v>
       </c>
       <c r="C54" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
       <c r="D54" t="s">
-        <v>175</v>
+        <v>313</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -2078,7 +2065,7 @@
         <v>104</v>
       </c>
       <c r="C55" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -2089,7 +2076,7 @@
         <v>106</v>
       </c>
       <c r="C56" t="s">
-        <v>178</v>
+        <v>315</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -2100,10 +2087,10 @@
         <v>108</v>
       </c>
       <c r="C57" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
       <c r="D57" t="s">
-        <v>175</v>
+        <v>313</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -2114,7 +2101,7 @@
         <v>110</v>
       </c>
       <c r="C58" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -2125,7 +2112,7 @@
         <v>112</v>
       </c>
       <c r="C59" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -2136,10 +2123,10 @@
         <v>114</v>
       </c>
       <c r="C60" t="s">
-        <v>177</v>
+        <v>312</v>
       </c>
       <c r="D60" t="s">
-        <v>170</v>
+        <v>317</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -2150,7 +2137,7 @@
         <v>116</v>
       </c>
       <c r="C61" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -2161,7 +2148,7 @@
         <v>118</v>
       </c>
       <c r="C62" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -2172,10 +2159,10 @@
         <v>120</v>
       </c>
       <c r="C63" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
       <c r="D63" t="s">
-        <v>175</v>
+        <v>313</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -2186,7 +2173,7 @@
         <v>122</v>
       </c>
       <c r="C64" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -2197,10 +2184,10 @@
         <v>124</v>
       </c>
       <c r="C65" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
       <c r="D65" t="s">
-        <v>170</v>
+        <v>317</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -2211,7 +2198,7 @@
         <v>126</v>
       </c>
       <c r="C66" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -2222,7 +2209,7 @@
         <v>128</v>
       </c>
       <c r="C67" t="s">
-        <v>170</v>
+        <v>317</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -2233,7 +2220,7 @@
         <v>130</v>
       </c>
       <c r="C68" t="s">
-        <v>170</v>
+        <v>317</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -2241,10 +2228,10 @@
         <v>131</v>
       </c>
       <c r="B69" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="C69" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -2252,10 +2239,10 @@
         <v>132</v>
       </c>
       <c r="B70" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="C70" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -2263,10 +2250,10 @@
         <v>133</v>
       </c>
       <c r="B71" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="C71" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -2274,13 +2261,13 @@
         <v>134</v>
       </c>
       <c r="B72" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="C72" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
       <c r="D72" t="s">
-        <v>175</v>
+        <v>313</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -2288,13 +2275,13 @@
         <v>135</v>
       </c>
       <c r="B73" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="C73" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
       <c r="D73" t="s">
-        <v>175</v>
+        <v>313</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -2302,13 +2289,13 @@
         <v>136</v>
       </c>
       <c r="B74" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="C74" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
       <c r="D74" t="s">
-        <v>175</v>
+        <v>313</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -2319,7 +2306,7 @@
         <v>138</v>
       </c>
       <c r="C75" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -2330,7 +2317,7 @@
         <v>140</v>
       </c>
       <c r="C76" t="s">
-        <v>169</v>
+        <v>312</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -2341,7 +2328,7 @@
         <v>142</v>
       </c>
       <c r="C77" t="s">
-        <v>171</v>
+        <v>319</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -2352,7 +2339,7 @@
         <v>144</v>
       </c>
       <c r="C78" t="s">
-        <v>171</v>
+        <v>319</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -2363,7 +2350,7 @@
         <v>146</v>
       </c>
       <c r="C79" t="s">
-        <v>171</v>
+        <v>319</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -2374,7 +2361,7 @@
         <v>148</v>
       </c>
       <c r="C80" t="s">
-        <v>171</v>
+        <v>319</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -2385,7 +2372,7 @@
         <v>150</v>
       </c>
       <c r="C81" t="s">
-        <v>171</v>
+        <v>319</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -2396,7 +2383,7 @@
         <v>152</v>
       </c>
       <c r="C82" t="s">
-        <v>174</v>
+        <v>320</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -2407,7 +2394,7 @@
         <v>154</v>
       </c>
       <c r="C83" t="s">
-        <v>174</v>
+        <v>320</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -2418,7 +2405,7 @@
         <v>156</v>
       </c>
       <c r="C84" t="s">
-        <v>174</v>
+        <v>320</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -2429,7 +2416,7 @@
         <v>158</v>
       </c>
       <c r="C85" t="s">
-        <v>174</v>
+        <v>320</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -2440,7 +2427,7 @@
         <v>160</v>
       </c>
       <c r="C86" t="s">
-        <v>174</v>
+        <v>320</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -2451,7 +2438,7 @@
         <v>162</v>
       </c>
       <c r="C87" t="s">
-        <v>174</v>
+        <v>320</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -2462,7 +2449,7 @@
         <v>164</v>
       </c>
       <c r="C88" t="s">
-        <v>174</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -2491,7 +2478,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2504,931 +2491,931 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="B3" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="C3" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="B4" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="C4" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="B5" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="C5" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="B6" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="C6" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="B7" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="C7" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="B8" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="C8" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="B9" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="C9" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="B10" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="C10" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="B11" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="C11" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="B12" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="C12" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="B13" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="C13" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="B14" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="C14" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="B15" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="C15" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="B16" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="C16" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="B17" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="C17" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="B18" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="C18" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="B19" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="C19" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="B20" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="C20" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="B21" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="C21" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="B22" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="C22" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="B23" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="C23" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="B24" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="C24" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="B25" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="C25" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="B26" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="C26" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="B27" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="C27" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="B28" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="C28" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="B29" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="C29" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="B30" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="C30" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="B31" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="C31" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="B32" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="C32" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="B33" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="C33" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="B34" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="C34" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="B35" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="C35" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="B36" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="C36" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="B37" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="C37" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="B38" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="C38" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="B39" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="C39" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="B40" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="C40" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="B41" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="C41" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="B42" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="C42" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="B43" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="C43" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="B44" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="C44" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="B45" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="C45" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="B46" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="C46" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="B47" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="C47" t="s">
-        <v>191</v>
+        <v>323</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="B48" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="C48" t="s">
-        <v>287</v>
+        <v>322</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="B49" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="C49" t="s">
-        <v>287</v>
+        <v>322</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="B50" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="C50" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="B51" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="C51" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="B52" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="C52" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="B53" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="C53" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="B54" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="C54" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="B55" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="C55" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="B56" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="C56" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
       <c r="B57" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="C57" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="B58" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="C58" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="B59" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="C59" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="B60" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="C60" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="B61" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="C61" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="B62" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="C62" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="B63" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="C63" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="B64" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="C64" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="B65" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="C65" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="B66" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="C66" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="B67" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="C67" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="B68" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="C68" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B69" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="C69" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="B70" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="C70" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="B71" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="C71" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="B72" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="C72" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="B73" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="C73" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="B74" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="C74" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="B75" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="C75" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="B76" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="C76" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="B77" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="C77" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="B78" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="C78" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="B79" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="C79" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="B80" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="C80" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
       <c r="B81" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="C81" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="B82" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="C82" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="B83" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="C83" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
       <c r="B84" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="C84" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="B85" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="C85" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="B86" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="C86" t="s">
-        <v>286</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit wiring branch connecting  and wiring command command bugs (#1114)
Co-authored-by: 汤永靖 <tangyongjing@thape.com.cn>
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/连线功能白名单.xlsx
+++ b/AutoLoader/Contents/Support/连线功能白名单.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="火灾报警" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="338">
   <si>
     <t>名称</t>
   </si>
@@ -1107,6 +1107,62 @@
   </si>
   <si>
     <t>平时照明布线</t>
+  </si>
+  <si>
+    <t>形状分类</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rectangle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rectangle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Capsule</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Square</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Square</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trapezoid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trapezoid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Circle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Circle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1149,10 +1205,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1434,10 +1493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D88"/>
+  <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1446,9 +1505,11 @@
     <col min="2" max="2" width="40.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.75" customWidth="1"/>
     <col min="4" max="4" width="21.75" customWidth="1"/>
+    <col min="5" max="5" width="12" style="2" customWidth="1"/>
+    <col min="6" max="9" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>168</v>
       </c>
@@ -1456,7 +1517,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>165</v>
       </c>
@@ -1469,8 +1530,23 @@
       <c r="D2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1480,8 +1556,23 @@
       <c r="C3" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F3" s="2">
+        <v>250</v>
+      </c>
+      <c r="G3" s="2">
+        <v>250</v>
+      </c>
+      <c r="H3" s="2">
+        <v>150</v>
+      </c>
+      <c r="I3" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1491,8 +1582,23 @@
       <c r="C4" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="F4" s="2">
+        <v>250</v>
+      </c>
+      <c r="G4" s="2">
+        <v>250</v>
+      </c>
+      <c r="H4" s="2">
+        <v>150</v>
+      </c>
+      <c r="I4" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1502,8 +1608,23 @@
       <c r="C5" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F5" s="2">
+        <v>150</v>
+      </c>
+      <c r="G5" s="2">
+        <v>150</v>
+      </c>
+      <c r="H5" s="2">
+        <v>150</v>
+      </c>
+      <c r="I5" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1513,8 +1634,23 @@
       <c r="C6" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F6" s="2">
+        <v>150</v>
+      </c>
+      <c r="G6" s="2">
+        <v>150</v>
+      </c>
+      <c r="H6" s="2">
+        <v>150</v>
+      </c>
+      <c r="I6" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1524,8 +1660,23 @@
       <c r="C7" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="F7" s="2">
+        <v>150</v>
+      </c>
+      <c r="G7" s="2">
+        <v>150</v>
+      </c>
+      <c r="H7" s="2">
+        <v>300</v>
+      </c>
+      <c r="I7" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1535,8 +1686,23 @@
       <c r="C8" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F8" s="2">
+        <v>250</v>
+      </c>
+      <c r="G8" s="2">
+        <v>250</v>
+      </c>
+      <c r="H8" s="2">
+        <v>150</v>
+      </c>
+      <c r="I8" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1546,8 +1712,23 @@
       <c r="C9" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F9" s="2">
+        <v>250</v>
+      </c>
+      <c r="G9" s="2">
+        <v>250</v>
+      </c>
+      <c r="H9" s="2">
+        <v>150</v>
+      </c>
+      <c r="I9" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1557,8 +1738,23 @@
       <c r="C10" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F10" s="2">
+        <v>250</v>
+      </c>
+      <c r="G10" s="2">
+        <v>250</v>
+      </c>
+      <c r="H10" s="2">
+        <v>150</v>
+      </c>
+      <c r="I10" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1568,8 +1764,23 @@
       <c r="C11" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F11" s="2">
+        <v>250</v>
+      </c>
+      <c r="G11" s="2">
+        <v>250</v>
+      </c>
+      <c r="H11" s="2">
+        <v>150</v>
+      </c>
+      <c r="I11" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1579,8 +1790,23 @@
       <c r="C12" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="F12" s="2">
+        <v>250</v>
+      </c>
+      <c r="G12" s="2">
+        <v>250</v>
+      </c>
+      <c r="H12" s="2">
+        <v>150</v>
+      </c>
+      <c r="I12" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1590,8 +1816,23 @@
       <c r="C13" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F13" s="2">
+        <v>150</v>
+      </c>
+      <c r="G13" s="2">
+        <v>150</v>
+      </c>
+      <c r="H13" s="2">
+        <v>150</v>
+      </c>
+      <c r="I13" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1601,8 +1842,23 @@
       <c r="C14" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F14" s="2">
+        <v>150</v>
+      </c>
+      <c r="G14" s="2">
+        <v>150</v>
+      </c>
+      <c r="H14" s="2">
+        <v>150</v>
+      </c>
+      <c r="I14" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1612,8 +1868,23 @@
       <c r="C15" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F15" s="2">
+        <v>150</v>
+      </c>
+      <c r="G15" s="2">
+        <v>150</v>
+      </c>
+      <c r="H15" s="2">
+        <v>150</v>
+      </c>
+      <c r="I15" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1623,8 +1894,23 @@
       <c r="C16" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F16" s="2">
+        <v>250</v>
+      </c>
+      <c r="G16" s="2">
+        <v>250</v>
+      </c>
+      <c r="H16" s="2">
+        <v>150</v>
+      </c>
+      <c r="I16" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1634,8 +1920,23 @@
       <c r="C17" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="F17" s="2">
+        <v>400</v>
+      </c>
+      <c r="G17" s="2">
+        <v>400</v>
+      </c>
+      <c r="H17" s="2">
+        <v>300</v>
+      </c>
+      <c r="I17" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -1645,8 +1946,23 @@
       <c r="C18" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="F18" s="2">
+        <v>400</v>
+      </c>
+      <c r="G18" s="2">
+        <v>400</v>
+      </c>
+      <c r="H18" s="2">
+        <v>300</v>
+      </c>
+      <c r="I18" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1656,8 +1972,23 @@
       <c r="C19" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="F19" s="2">
+        <v>400</v>
+      </c>
+      <c r="G19" s="2">
+        <v>400</v>
+      </c>
+      <c r="H19" s="2">
+        <v>300</v>
+      </c>
+      <c r="I19" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1670,8 +2001,23 @@
       <c r="D20" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F20" s="2">
+        <v>250</v>
+      </c>
+      <c r="G20" s="2">
+        <v>250</v>
+      </c>
+      <c r="H20" s="2">
+        <v>150</v>
+      </c>
+      <c r="I20" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -1681,8 +2027,23 @@
       <c r="C21" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F21" s="2">
+        <v>250</v>
+      </c>
+      <c r="G21" s="2">
+        <v>250</v>
+      </c>
+      <c r="H21" s="2">
+        <v>150</v>
+      </c>
+      <c r="I21" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -1692,8 +2053,23 @@
       <c r="C22" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F22" s="2">
+        <v>250</v>
+      </c>
+      <c r="G22" s="2">
+        <v>250</v>
+      </c>
+      <c r="H22" s="2">
+        <v>150</v>
+      </c>
+      <c r="I22" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -1703,8 +2079,23 @@
       <c r="C23" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F23" s="2">
+        <v>250</v>
+      </c>
+      <c r="G23" s="2">
+        <v>250</v>
+      </c>
+      <c r="H23" s="2">
+        <v>150</v>
+      </c>
+      <c r="I23" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -1714,8 +2105,23 @@
       <c r="C24" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F24" s="2">
+        <v>150</v>
+      </c>
+      <c r="G24" s="2">
+        <v>150</v>
+      </c>
+      <c r="H24" s="2">
+        <v>150</v>
+      </c>
+      <c r="I24" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -1725,8 +2131,23 @@
       <c r="C25" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F25" s="2">
+        <v>150</v>
+      </c>
+      <c r="G25" s="2">
+        <v>150</v>
+      </c>
+      <c r="H25" s="2">
+        <v>150</v>
+      </c>
+      <c r="I25" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -1736,8 +2157,23 @@
       <c r="C26" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F26" s="2">
+        <v>150</v>
+      </c>
+      <c r="G26" s="2">
+        <v>150</v>
+      </c>
+      <c r="H26" s="2">
+        <v>150</v>
+      </c>
+      <c r="I26" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -1750,8 +2186,23 @@
       <c r="D27" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F27" s="2">
+        <v>150</v>
+      </c>
+      <c r="G27" s="2">
+        <v>150</v>
+      </c>
+      <c r="H27" s="2">
+        <v>150</v>
+      </c>
+      <c r="I27" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>51</v>
       </c>
@@ -1761,8 +2212,23 @@
       <c r="C28" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F28" s="2">
+        <v>150</v>
+      </c>
+      <c r="G28" s="2">
+        <v>150</v>
+      </c>
+      <c r="H28" s="2">
+        <v>150</v>
+      </c>
+      <c r="I28" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -1772,8 +2238,23 @@
       <c r="C29" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="F29" s="2">
+        <v>400</v>
+      </c>
+      <c r="G29" s="2">
+        <v>400</v>
+      </c>
+      <c r="H29" s="2">
+        <v>300</v>
+      </c>
+      <c r="I29" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -1783,8 +2264,23 @@
       <c r="C30" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F30" s="2">
+        <v>150</v>
+      </c>
+      <c r="G30" s="2">
+        <v>150</v>
+      </c>
+      <c r="H30" s="2">
+        <v>300</v>
+      </c>
+      <c r="I30" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>57</v>
       </c>
@@ -1794,8 +2290,23 @@
       <c r="C31" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F31" s="2">
+        <v>150</v>
+      </c>
+      <c r="G31" s="2">
+        <v>150</v>
+      </c>
+      <c r="H31" s="2">
+        <v>150</v>
+      </c>
+      <c r="I31" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>59</v>
       </c>
@@ -1805,8 +2316,23 @@
       <c r="C32" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="F32" s="2">
+        <v>150</v>
+      </c>
+      <c r="G32" s="2">
+        <v>150</v>
+      </c>
+      <c r="H32" s="2">
+        <v>150</v>
+      </c>
+      <c r="I32" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>61</v>
       </c>
@@ -1816,8 +2342,23 @@
       <c r="C33" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F33" s="2">
+        <v>150</v>
+      </c>
+      <c r="G33" s="2">
+        <v>150</v>
+      </c>
+      <c r="H33" s="2">
+        <v>150</v>
+      </c>
+      <c r="I33" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -1827,8 +2368,23 @@
       <c r="C34" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F34" s="2">
+        <v>150</v>
+      </c>
+      <c r="G34" s="2">
+        <v>150</v>
+      </c>
+      <c r="H34" s="2">
+        <v>150</v>
+      </c>
+      <c r="I34" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>65</v>
       </c>
@@ -1838,8 +2394,23 @@
       <c r="C35" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F35" s="2">
+        <v>150</v>
+      </c>
+      <c r="G35" s="2">
+        <v>150</v>
+      </c>
+      <c r="H35" s="2">
+        <v>150</v>
+      </c>
+      <c r="I35" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>67</v>
       </c>
@@ -1849,8 +2420,23 @@
       <c r="C36" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="F36" s="2">
+        <v>400</v>
+      </c>
+      <c r="G36" s="2">
+        <v>400</v>
+      </c>
+      <c r="H36" s="2">
+        <v>300</v>
+      </c>
+      <c r="I36" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -1860,8 +2446,23 @@
       <c r="C37" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F37" s="2">
+        <v>150</v>
+      </c>
+      <c r="G37" s="2">
+        <v>150</v>
+      </c>
+      <c r="H37" s="2">
+        <v>300</v>
+      </c>
+      <c r="I37" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>71</v>
       </c>
@@ -1871,8 +2472,23 @@
       <c r="C38" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F38" s="2">
+        <v>150</v>
+      </c>
+      <c r="G38" s="2">
+        <v>150</v>
+      </c>
+      <c r="H38" s="2">
+        <v>150</v>
+      </c>
+      <c r="I38" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>73</v>
       </c>
@@ -1882,8 +2498,23 @@
       <c r="C39" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F39" s="2">
+        <v>150</v>
+      </c>
+      <c r="G39" s="2">
+        <v>150</v>
+      </c>
+      <c r="H39" s="2">
+        <v>150</v>
+      </c>
+      <c r="I39" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>75</v>
       </c>
@@ -1893,8 +2524,23 @@
       <c r="C40" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F40" s="2">
+        <v>250</v>
+      </c>
+      <c r="G40" s="2">
+        <v>250</v>
+      </c>
+      <c r="H40" s="2">
+        <v>150</v>
+      </c>
+      <c r="I40" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>77</v>
       </c>
@@ -1907,8 +2553,23 @@
       <c r="D41" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F41" s="2">
+        <v>150</v>
+      </c>
+      <c r="G41" s="2">
+        <v>150</v>
+      </c>
+      <c r="H41" s="2">
+        <v>150</v>
+      </c>
+      <c r="I41" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>79</v>
       </c>
@@ -1918,8 +2579,23 @@
       <c r="C42" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F42" s="2">
+        <v>150</v>
+      </c>
+      <c r="G42" s="2">
+        <v>150</v>
+      </c>
+      <c r="H42" s="2">
+        <v>150</v>
+      </c>
+      <c r="I42" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>81</v>
       </c>
@@ -1929,8 +2605,23 @@
       <c r="C43" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F43" s="2">
+        <v>150</v>
+      </c>
+      <c r="G43" s="2">
+        <v>150</v>
+      </c>
+      <c r="H43" s="2">
+        <v>150</v>
+      </c>
+      <c r="I43" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>83</v>
       </c>
@@ -1940,8 +2631,23 @@
       <c r="C44" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F44" s="2">
+        <v>150</v>
+      </c>
+      <c r="G44" s="2">
+        <v>150</v>
+      </c>
+      <c r="H44" s="2">
+        <v>150</v>
+      </c>
+      <c r="I44" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -1951,8 +2657,23 @@
       <c r="C45" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="F45" s="2">
+        <v>400</v>
+      </c>
+      <c r="G45" s="2">
+        <v>400</v>
+      </c>
+      <c r="H45" s="2">
+        <v>300</v>
+      </c>
+      <c r="I45" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>87</v>
       </c>
@@ -1962,8 +2683,23 @@
       <c r="C46" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="F46" s="2">
+        <v>400</v>
+      </c>
+      <c r="G46" s="2">
+        <v>400</v>
+      </c>
+      <c r="H46" s="2">
+        <v>300</v>
+      </c>
+      <c r="I46" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>89</v>
       </c>
@@ -1973,8 +2709,23 @@
       <c r="C47" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="F47" s="2">
+        <v>400</v>
+      </c>
+      <c r="G47" s="2">
+        <v>400</v>
+      </c>
+      <c r="H47" s="2">
+        <v>300</v>
+      </c>
+      <c r="I47" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>91</v>
       </c>
@@ -1984,8 +2735,23 @@
       <c r="C48" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="F48" s="2">
+        <v>400</v>
+      </c>
+      <c r="G48" s="2">
+        <v>400</v>
+      </c>
+      <c r="H48" s="2">
+        <v>300</v>
+      </c>
+      <c r="I48" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>93</v>
       </c>
@@ -1995,8 +2761,23 @@
       <c r="C49" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="F49" s="2">
+        <v>400</v>
+      </c>
+      <c r="G49" s="2">
+        <v>400</v>
+      </c>
+      <c r="H49" s="2">
+        <v>300</v>
+      </c>
+      <c r="I49" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>94</v>
       </c>
@@ -2006,8 +2787,23 @@
       <c r="C50" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="F50" s="2">
+        <v>400</v>
+      </c>
+      <c r="G50" s="2">
+        <v>400</v>
+      </c>
+      <c r="H50" s="2">
+        <v>300</v>
+      </c>
+      <c r="I50" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>95</v>
       </c>
@@ -2017,8 +2813,23 @@
       <c r="C51" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F51" s="2">
+        <v>150</v>
+      </c>
+      <c r="G51" s="2">
+        <v>150</v>
+      </c>
+      <c r="H51" s="2">
+        <v>150</v>
+      </c>
+      <c r="I51" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>97</v>
       </c>
@@ -2028,8 +2839,23 @@
       <c r="C52" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F52" s="2">
+        <v>150</v>
+      </c>
+      <c r="G52" s="2">
+        <v>150</v>
+      </c>
+      <c r="H52" s="2">
+        <v>150</v>
+      </c>
+      <c r="I52" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>99</v>
       </c>
@@ -2042,8 +2868,23 @@
       <c r="D53" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F53" s="2">
+        <v>150</v>
+      </c>
+      <c r="G53" s="2">
+        <v>150</v>
+      </c>
+      <c r="H53" s="2">
+        <v>150</v>
+      </c>
+      <c r="I53" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>101</v>
       </c>
@@ -2056,8 +2897,23 @@
       <c r="D54" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F54" s="2">
+        <v>150</v>
+      </c>
+      <c r="G54" s="2">
+        <v>150</v>
+      </c>
+      <c r="H54" s="2">
+        <v>150</v>
+      </c>
+      <c r="I54" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>103</v>
       </c>
@@ -2067,8 +2923,23 @@
       <c r="C55" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F55" s="2">
+        <v>150</v>
+      </c>
+      <c r="G55" s="2">
+        <v>150</v>
+      </c>
+      <c r="H55" s="2">
+        <v>150</v>
+      </c>
+      <c r="I55" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>105</v>
       </c>
@@ -2078,8 +2949,23 @@
       <c r="C56" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F56" s="2">
+        <v>150</v>
+      </c>
+      <c r="G56" s="2">
+        <v>150</v>
+      </c>
+      <c r="H56" s="2">
+        <v>150</v>
+      </c>
+      <c r="I56" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>107</v>
       </c>
@@ -2092,8 +2978,23 @@
       <c r="D57" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F57" s="2">
+        <v>150</v>
+      </c>
+      <c r="G57" s="2">
+        <v>150</v>
+      </c>
+      <c r="H57" s="2">
+        <v>150</v>
+      </c>
+      <c r="I57" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>109</v>
       </c>
@@ -2103,8 +3004,23 @@
       <c r="C58" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F58" s="2">
+        <v>150</v>
+      </c>
+      <c r="G58" s="2">
+        <v>150</v>
+      </c>
+      <c r="H58" s="2">
+        <v>150</v>
+      </c>
+      <c r="I58" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>111</v>
       </c>
@@ -2114,8 +3030,23 @@
       <c r="C59" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F59" s="2">
+        <v>150</v>
+      </c>
+      <c r="G59" s="2">
+        <v>150</v>
+      </c>
+      <c r="H59" s="2">
+        <v>150</v>
+      </c>
+      <c r="I59" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>113</v>
       </c>
@@ -2128,8 +3059,23 @@
       <c r="D60" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F60" s="2">
+        <v>150</v>
+      </c>
+      <c r="G60" s="2">
+        <v>150</v>
+      </c>
+      <c r="H60" s="2">
+        <v>150</v>
+      </c>
+      <c r="I60" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>115</v>
       </c>
@@ -2139,8 +3085,23 @@
       <c r="C61" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F61" s="2">
+        <v>300</v>
+      </c>
+      <c r="G61" s="2">
+        <v>300</v>
+      </c>
+      <c r="H61" s="2">
+        <v>150</v>
+      </c>
+      <c r="I61" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>117</v>
       </c>
@@ -2150,8 +3111,23 @@
       <c r="C62" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="F62" s="2">
+        <v>150</v>
+      </c>
+      <c r="G62" s="2">
+        <v>150</v>
+      </c>
+      <c r="H62" s="2">
+        <v>150</v>
+      </c>
+      <c r="I62" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>119</v>
       </c>
@@ -2164,8 +3140,23 @@
       <c r="D63" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F63" s="2">
+        <v>150</v>
+      </c>
+      <c r="G63" s="2">
+        <v>150</v>
+      </c>
+      <c r="H63" s="2">
+        <v>150</v>
+      </c>
+      <c r="I63" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>121</v>
       </c>
@@ -2175,8 +3166,23 @@
       <c r="C64" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F64" s="2">
+        <v>150</v>
+      </c>
+      <c r="G64" s="2">
+        <v>150</v>
+      </c>
+      <c r="H64" s="2">
+        <v>150</v>
+      </c>
+      <c r="I64" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>123</v>
       </c>
@@ -2189,8 +3195,23 @@
       <c r="D65" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F65" s="2">
+        <v>300</v>
+      </c>
+      <c r="G65" s="2">
+        <v>300</v>
+      </c>
+      <c r="H65" s="2">
+        <v>150</v>
+      </c>
+      <c r="I65" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>125</v>
       </c>
@@ -2200,8 +3221,23 @@
       <c r="C66" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F66" s="2">
+        <v>150</v>
+      </c>
+      <c r="G66" s="2">
+        <v>150</v>
+      </c>
+      <c r="H66" s="2">
+        <v>150</v>
+      </c>
+      <c r="I66" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>127</v>
       </c>
@@ -2211,8 +3247,23 @@
       <c r="C67" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="F67" s="2">
+        <v>150</v>
+      </c>
+      <c r="G67" s="2">
+        <v>150</v>
+      </c>
+      <c r="H67" s="2">
+        <v>150</v>
+      </c>
+      <c r="I67" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>129</v>
       </c>
@@ -2222,8 +3273,23 @@
       <c r="C68" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F68" s="2">
+        <v>150</v>
+      </c>
+      <c r="G68" s="2">
+        <v>150</v>
+      </c>
+      <c r="H68" s="2">
+        <v>150</v>
+      </c>
+      <c r="I68" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>131</v>
       </c>
@@ -2233,8 +3299,23 @@
       <c r="C69" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F69" s="2">
+        <v>150</v>
+      </c>
+      <c r="G69" s="2">
+        <v>150</v>
+      </c>
+      <c r="H69" s="2">
+        <v>150</v>
+      </c>
+      <c r="I69" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>132</v>
       </c>
@@ -2244,8 +3325,23 @@
       <c r="C70" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F70" s="2">
+        <v>150</v>
+      </c>
+      <c r="G70" s="2">
+        <v>150</v>
+      </c>
+      <c r="H70" s="2">
+        <v>150</v>
+      </c>
+      <c r="I70" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>133</v>
       </c>
@@ -2255,8 +3351,23 @@
       <c r="C71" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F71" s="2">
+        <v>150</v>
+      </c>
+      <c r="G71" s="2">
+        <v>150</v>
+      </c>
+      <c r="H71" s="2">
+        <v>150</v>
+      </c>
+      <c r="I71" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>134</v>
       </c>
@@ -2269,8 +3380,23 @@
       <c r="D72" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F72" s="2">
+        <v>150</v>
+      </c>
+      <c r="G72" s="2">
+        <v>150</v>
+      </c>
+      <c r="H72" s="2">
+        <v>150</v>
+      </c>
+      <c r="I72" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>135</v>
       </c>
@@ -2283,8 +3409,23 @@
       <c r="D73" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F73" s="2">
+        <v>150</v>
+      </c>
+      <c r="G73" s="2">
+        <v>150</v>
+      </c>
+      <c r="H73" s="2">
+        <v>150</v>
+      </c>
+      <c r="I73" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>136</v>
       </c>
@@ -2297,8 +3438,23 @@
       <c r="D74" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F74" s="2">
+        <v>150</v>
+      </c>
+      <c r="G74" s="2">
+        <v>150</v>
+      </c>
+      <c r="H74" s="2">
+        <v>150</v>
+      </c>
+      <c r="I74" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>137</v>
       </c>
@@ -2308,8 +3464,23 @@
       <c r="C75" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="F75" s="2">
+        <v>250</v>
+      </c>
+      <c r="G75" s="2">
+        <v>250</v>
+      </c>
+      <c r="H75" s="2">
+        <v>150</v>
+      </c>
+      <c r="I75" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>139</v>
       </c>
@@ -2319,8 +3490,23 @@
       <c r="C76" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F76" s="2">
+        <v>250</v>
+      </c>
+      <c r="G76" s="2">
+        <v>250</v>
+      </c>
+      <c r="H76" s="2">
+        <v>150</v>
+      </c>
+      <c r="I76" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>141</v>
       </c>
@@ -2330,8 +3516,23 @@
       <c r="C77" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F77" s="2">
+        <v>250</v>
+      </c>
+      <c r="G77" s="2">
+        <v>250</v>
+      </c>
+      <c r="H77" s="2">
+        <v>150</v>
+      </c>
+      <c r="I77" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>143</v>
       </c>
@@ -2341,8 +3542,23 @@
       <c r="C78" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F78" s="2">
+        <v>150</v>
+      </c>
+      <c r="G78" s="2">
+        <v>150</v>
+      </c>
+      <c r="H78" s="2">
+        <v>150</v>
+      </c>
+      <c r="I78" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>145</v>
       </c>
@@ -2352,8 +3568,23 @@
       <c r="C79" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="F79" s="2">
+        <v>250</v>
+      </c>
+      <c r="G79" s="2">
+        <v>250</v>
+      </c>
+      <c r="H79" s="2">
+        <v>150</v>
+      </c>
+      <c r="I79" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>147</v>
       </c>
@@ -2363,8 +3594,23 @@
       <c r="C80" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E80" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F80" s="2">
+        <v>150</v>
+      </c>
+      <c r="G80" s="2">
+        <v>150</v>
+      </c>
+      <c r="H80" s="2">
+        <v>150</v>
+      </c>
+      <c r="I80" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>149</v>
       </c>
@@ -2374,8 +3620,23 @@
       <c r="C81" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E81" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="F81" s="2">
+        <v>150</v>
+      </c>
+      <c r="G81" s="2">
+        <v>150</v>
+      </c>
+      <c r="H81" s="2">
+        <v>150</v>
+      </c>
+      <c r="I81" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>151</v>
       </c>
@@ -2385,8 +3646,23 @@
       <c r="C82" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E82" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F82" s="2">
+        <v>250</v>
+      </c>
+      <c r="G82" s="2">
+        <v>250</v>
+      </c>
+      <c r="H82" s="2">
+        <v>150</v>
+      </c>
+      <c r="I82" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>153</v>
       </c>
@@ -2396,8 +3672,23 @@
       <c r="C83" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E83" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F83" s="2">
+        <v>250</v>
+      </c>
+      <c r="G83" s="2">
+        <v>250</v>
+      </c>
+      <c r="H83" s="2">
+        <v>150</v>
+      </c>
+      <c r="I83" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>155</v>
       </c>
@@ -2407,8 +3698,23 @@
       <c r="C84" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E84" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F84" s="2">
+        <v>250</v>
+      </c>
+      <c r="G84" s="2">
+        <v>250</v>
+      </c>
+      <c r="H84" s="2">
+        <v>150</v>
+      </c>
+      <c r="I84" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>157</v>
       </c>
@@ -2418,8 +3724,23 @@
       <c r="C85" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E85" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="F85" s="2">
+        <v>250</v>
+      </c>
+      <c r="G85" s="2">
+        <v>250</v>
+      </c>
+      <c r="H85" s="2">
+        <v>150</v>
+      </c>
+      <c r="I85" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>159</v>
       </c>
@@ -2429,8 +3750,23 @@
       <c r="C86" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E86" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F86" s="2">
+        <v>150</v>
+      </c>
+      <c r="G86" s="2">
+        <v>150</v>
+      </c>
+      <c r="H86" s="2">
+        <v>150</v>
+      </c>
+      <c r="I86" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>161</v>
       </c>
@@ -2440,8 +3776,23 @@
       <c r="C87" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E87" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F87" s="2">
+        <v>150</v>
+      </c>
+      <c r="G87" s="2">
+        <v>150</v>
+      </c>
+      <c r="H87" s="2">
+        <v>150</v>
+      </c>
+      <c r="I87" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>163</v>
       </c>
@@ -2450,6 +3801,21 @@
       </c>
       <c r="C88" t="s">
         <v>320</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F88" s="2">
+        <v>150</v>
+      </c>
+      <c r="G88" s="2">
+        <v>150</v>
+      </c>
+      <c r="H88" s="2">
+        <v>150</v>
+      </c>
+      <c r="I88" s="2">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2463,27 +3829,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C86"/>
+  <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.625" customWidth="1"/>
-    <col min="3" max="3" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>169</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>165</v>
       </c>
@@ -2493,8 +3859,23 @@
       <c r="C2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>170</v>
       </c>
@@ -2504,8 +3885,23 @@
       <c r="C3" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E3" s="2">
+        <v>550</v>
+      </c>
+      <c r="F3" s="2">
+        <v>550</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>171</v>
       </c>
@@ -2515,8 +3911,23 @@
       <c r="C4" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E4" s="2">
+        <v>550</v>
+      </c>
+      <c r="F4" s="2">
+        <v>550</v>
+      </c>
+      <c r="G4" s="2">
+        <v>50</v>
+      </c>
+      <c r="H4" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>172</v>
       </c>
@@ -2526,8 +3937,23 @@
       <c r="C5" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E5" s="2">
+        <v>550</v>
+      </c>
+      <c r="F5" s="2">
+        <v>550</v>
+      </c>
+      <c r="G5" s="2">
+        <v>100</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>173</v>
       </c>
@@ -2537,8 +3963,23 @@
       <c r="C6" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E6" s="2">
+        <v>550</v>
+      </c>
+      <c r="F6" s="2">
+        <v>550</v>
+      </c>
+      <c r="G6" s="2">
+        <v>75</v>
+      </c>
+      <c r="H6" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>174</v>
       </c>
@@ -2548,8 +3989,23 @@
       <c r="C7" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E7" s="2">
+        <v>550</v>
+      </c>
+      <c r="F7" s="2">
+        <v>550</v>
+      </c>
+      <c r="G7" s="2">
+        <v>150</v>
+      </c>
+      <c r="H7" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>175</v>
       </c>
@@ -2559,8 +4015,23 @@
       <c r="C8" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E8" s="2">
+        <v>550</v>
+      </c>
+      <c r="F8" s="2">
+        <v>550</v>
+      </c>
+      <c r="G8" s="2">
+        <v>300</v>
+      </c>
+      <c r="H8" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>176</v>
       </c>
@@ -2570,8 +4041,23 @@
       <c r="C9" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E9" s="2">
+        <v>550</v>
+      </c>
+      <c r="F9" s="2">
+        <v>550</v>
+      </c>
+      <c r="G9" s="2">
+        <v>75</v>
+      </c>
+      <c r="H9" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>177</v>
       </c>
@@ -2581,8 +4067,23 @@
       <c r="C10" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E10" s="2">
+        <v>550</v>
+      </c>
+      <c r="F10" s="2">
+        <v>550</v>
+      </c>
+      <c r="G10" s="2">
+        <v>150</v>
+      </c>
+      <c r="H10" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>192</v>
       </c>
@@ -2592,8 +4093,23 @@
       <c r="C11" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E11" s="2">
+        <v>550</v>
+      </c>
+      <c r="F11" s="2">
+        <v>550</v>
+      </c>
+      <c r="G11" s="2">
+        <v>150</v>
+      </c>
+      <c r="H11" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>187</v>
       </c>
@@ -2603,8 +4119,23 @@
       <c r="C12" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E12" s="2">
+        <v>550</v>
+      </c>
+      <c r="F12" s="2">
+        <v>550</v>
+      </c>
+      <c r="G12" s="2">
+        <v>150</v>
+      </c>
+      <c r="H12" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>195</v>
       </c>
@@ -2614,8 +4145,23 @@
       <c r="C13" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E13" s="2">
+        <v>550</v>
+      </c>
+      <c r="F13" s="2">
+        <v>550</v>
+      </c>
+      <c r="G13" s="2">
+        <v>300</v>
+      </c>
+      <c r="H13" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>188</v>
       </c>
@@ -2625,8 +4171,23 @@
       <c r="C14" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E14" s="2">
+        <v>550</v>
+      </c>
+      <c r="F14" s="2">
+        <v>550</v>
+      </c>
+      <c r="G14" s="2">
+        <v>300</v>
+      </c>
+      <c r="H14" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>196</v>
       </c>
@@ -2636,8 +4197,23 @@
       <c r="C15" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E15" s="2">
+        <v>300</v>
+      </c>
+      <c r="F15" s="2">
+        <v>300</v>
+      </c>
+      <c r="G15" s="2">
+        <v>300</v>
+      </c>
+      <c r="H15" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>189</v>
       </c>
@@ -2647,8 +4223,23 @@
       <c r="C16" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E16" s="2">
+        <v>300</v>
+      </c>
+      <c r="F16" s="2">
+        <v>300</v>
+      </c>
+      <c r="G16" s="2">
+        <v>300</v>
+      </c>
+      <c r="H16" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>220</v>
       </c>
@@ -2658,8 +4249,23 @@
       <c r="C17" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="E17" s="2">
+        <v>100</v>
+      </c>
+      <c r="F17" s="2">
+        <v>100</v>
+      </c>
+      <c r="G17" s="2">
+        <v>100</v>
+      </c>
+      <c r="H17" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>221</v>
       </c>
@@ -2669,8 +4275,23 @@
       <c r="C18" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="E18" s="2">
+        <v>100</v>
+      </c>
+      <c r="F18" s="2">
+        <v>100</v>
+      </c>
+      <c r="G18" s="2">
+        <v>100</v>
+      </c>
+      <c r="H18" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>222</v>
       </c>
@@ -2680,8 +4301,23 @@
       <c r="C19" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="E19" s="2">
+        <v>75</v>
+      </c>
+      <c r="F19" s="2">
+        <v>75</v>
+      </c>
+      <c r="G19" s="2">
+        <v>75</v>
+      </c>
+      <c r="H19" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>224</v>
       </c>
@@ -2691,8 +4327,23 @@
       <c r="C20" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="E20" s="2">
+        <v>75</v>
+      </c>
+      <c r="F20" s="2">
+        <v>75</v>
+      </c>
+      <c r="G20" s="2">
+        <v>75</v>
+      </c>
+      <c r="H20" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>223</v>
       </c>
@@ -2702,8 +4353,23 @@
       <c r="C21" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="E21" s="2">
+        <v>50</v>
+      </c>
+      <c r="F21" s="2">
+        <v>50</v>
+      </c>
+      <c r="G21" s="2">
+        <v>50</v>
+      </c>
+      <c r="H21" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>207</v>
       </c>
@@ -2713,8 +4379,23 @@
       <c r="C22" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="E22" s="2">
+        <v>150</v>
+      </c>
+      <c r="F22" s="2">
+        <v>150</v>
+      </c>
+      <c r="G22" s="2">
+        <v>150</v>
+      </c>
+      <c r="H22" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>197</v>
       </c>
@@ -2724,8 +4405,23 @@
       <c r="C23" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E23" s="2">
+        <v>150</v>
+      </c>
+      <c r="F23" s="2">
+        <v>150</v>
+      </c>
+      <c r="G23" s="2">
+        <v>150</v>
+      </c>
+      <c r="H23" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>198</v>
       </c>
@@ -2735,8 +4431,23 @@
       <c r="C24" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E24" s="2">
+        <v>150</v>
+      </c>
+      <c r="F24" s="2">
+        <v>150</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>203</v>
       </c>
@@ -2746,8 +4457,23 @@
       <c r="C25" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E25" s="2">
+        <v>150</v>
+      </c>
+      <c r="F25" s="2">
+        <v>150</v>
+      </c>
+      <c r="G25" s="2">
+        <v>150</v>
+      </c>
+      <c r="H25" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>217</v>
       </c>
@@ -2757,8 +4483,23 @@
       <c r="C26" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E26" s="2">
+        <v>150</v>
+      </c>
+      <c r="F26" s="2">
+        <v>150</v>
+      </c>
+      <c r="G26" s="2">
+        <v>150</v>
+      </c>
+      <c r="H26" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>201</v>
       </c>
@@ -2768,8 +4509,23 @@
       <c r="C27" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E27" s="2">
+        <v>150</v>
+      </c>
+      <c r="F27" s="2">
+        <v>150</v>
+      </c>
+      <c r="G27" s="2">
+        <v>150</v>
+      </c>
+      <c r="H27" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>202</v>
       </c>
@@ -2779,8 +4535,23 @@
       <c r="C28" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E28" s="2">
+        <v>150</v>
+      </c>
+      <c r="F28" s="2">
+        <v>150</v>
+      </c>
+      <c r="G28" s="2">
+        <v>150</v>
+      </c>
+      <c r="H28" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>227</v>
       </c>
@@ -2790,8 +4561,23 @@
       <c r="C29" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E29" s="2">
+        <v>250</v>
+      </c>
+      <c r="F29" s="2">
+        <v>250</v>
+      </c>
+      <c r="G29" s="2">
+        <v>50</v>
+      </c>
+      <c r="H29" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>212</v>
       </c>
@@ -2801,8 +4587,23 @@
       <c r="C30" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E30" s="2">
+        <v>150</v>
+      </c>
+      <c r="F30" s="2">
+        <v>150</v>
+      </c>
+      <c r="G30" s="2">
+        <v>75</v>
+      </c>
+      <c r="H30" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>213</v>
       </c>
@@ -2812,8 +4613,23 @@
       <c r="C31" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E31" s="2">
+        <v>150</v>
+      </c>
+      <c r="F31" s="2">
+        <v>150</v>
+      </c>
+      <c r="G31" s="2">
+        <v>75</v>
+      </c>
+      <c r="H31" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>209</v>
       </c>
@@ -2823,8 +4639,27 @@
       <c r="C32" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" ref="E32:H33" si="0">300/SQRT(2)</f>
+        <v>212.13203435596424</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="0"/>
+        <v>212.13203435596424</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="0"/>
+        <v>212.13203435596424</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="0"/>
+        <v>212.13203435596424</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>210</v>
       </c>
@@ -2834,8 +4669,27 @@
       <c r="C33" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="0"/>
+        <v>212.13203435596424</v>
+      </c>
+      <c r="F33" s="2">
+        <f t="shared" si="0"/>
+        <v>212.13203435596424</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="0"/>
+        <v>212.13203435596424</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="0"/>
+        <v>212.13203435596424</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>219</v>
       </c>
@@ -2845,8 +4699,23 @@
       <c r="C34" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E34" s="2">
+        <v>150</v>
+      </c>
+      <c r="F34" s="2">
+        <v>150</v>
+      </c>
+      <c r="G34" s="2">
+        <v>150</v>
+      </c>
+      <c r="H34" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>237</v>
       </c>
@@ -2856,8 +4725,23 @@
       <c r="C35" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E35" s="2">
+        <v>150</v>
+      </c>
+      <c r="F35" s="2">
+        <v>150</v>
+      </c>
+      <c r="G35" s="2">
+        <v>150</v>
+      </c>
+      <c r="H35" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>238</v>
       </c>
@@ -2867,8 +4751,23 @@
       <c r="C36" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E36" s="2">
+        <v>150</v>
+      </c>
+      <c r="F36" s="2">
+        <v>150</v>
+      </c>
+      <c r="G36" s="2">
+        <v>150</v>
+      </c>
+      <c r="H36" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>231</v>
       </c>
@@ -2878,8 +4777,23 @@
       <c r="C37" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E37" s="2">
+        <v>50</v>
+      </c>
+      <c r="F37" s="2">
+        <v>50</v>
+      </c>
+      <c r="G37" s="2">
+        <v>50</v>
+      </c>
+      <c r="H37" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>232</v>
       </c>
@@ -2889,8 +4803,23 @@
       <c r="C38" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E38" s="2">
+        <v>50</v>
+      </c>
+      <c r="F38" s="2">
+        <v>50</v>
+      </c>
+      <c r="G38" s="2">
+        <v>50</v>
+      </c>
+      <c r="H38" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>233</v>
       </c>
@@ -2900,8 +4829,23 @@
       <c r="C39" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E39" s="2">
+        <v>50</v>
+      </c>
+      <c r="F39" s="2">
+        <v>50</v>
+      </c>
+      <c r="G39" s="2">
+        <v>50</v>
+      </c>
+      <c r="H39" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>229</v>
       </c>
@@ -2911,8 +4855,23 @@
       <c r="C40" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E40" s="2">
+        <v>150</v>
+      </c>
+      <c r="F40" s="2">
+        <v>150</v>
+      </c>
+      <c r="G40" s="2">
+        <v>150</v>
+      </c>
+      <c r="H40" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>241</v>
       </c>
@@ -2922,8 +4881,23 @@
       <c r="C41" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E41" s="2">
+        <v>150</v>
+      </c>
+      <c r="F41" s="2">
+        <v>150</v>
+      </c>
+      <c r="G41" s="2">
+        <v>125</v>
+      </c>
+      <c r="H41" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>242</v>
       </c>
@@ -2933,8 +4907,23 @@
       <c r="C42" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E42" s="2">
+        <v>100</v>
+      </c>
+      <c r="F42" s="2">
+        <v>100</v>
+      </c>
+      <c r="G42" s="2">
+        <v>200</v>
+      </c>
+      <c r="H42" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>245</v>
       </c>
@@ -2944,8 +4933,23 @@
       <c r="C43" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E43" s="2">
+        <v>150</v>
+      </c>
+      <c r="F43" s="2">
+        <v>150</v>
+      </c>
+      <c r="G43" s="2">
+        <v>150</v>
+      </c>
+      <c r="H43" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>246</v>
       </c>
@@ -2955,8 +4959,23 @@
       <c r="C44" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E44" s="2">
+        <v>150</v>
+      </c>
+      <c r="F44" s="2">
+        <v>150</v>
+      </c>
+      <c r="G44" s="2">
+        <v>150</v>
+      </c>
+      <c r="H44" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>247</v>
       </c>
@@ -2966,8 +4985,23 @@
       <c r="C45" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E45" s="2">
+        <v>150</v>
+      </c>
+      <c r="F45" s="2">
+        <v>150</v>
+      </c>
+      <c r="G45" s="2">
+        <v>150</v>
+      </c>
+      <c r="H45" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>248</v>
       </c>
@@ -2977,8 +5011,23 @@
       <c r="C46" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E46" s="2">
+        <v>150</v>
+      </c>
+      <c r="F46" s="2">
+        <v>150</v>
+      </c>
+      <c r="G46" s="2">
+        <v>150</v>
+      </c>
+      <c r="H46" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>249</v>
       </c>
@@ -2988,8 +5037,23 @@
       <c r="C47" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E47" s="2">
+        <v>150</v>
+      </c>
+      <c r="F47" s="2">
+        <v>150</v>
+      </c>
+      <c r="G47" s="2">
+        <v>150</v>
+      </c>
+      <c r="H47" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>257</v>
       </c>
@@ -2999,8 +5063,23 @@
       <c r="C48" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E48" s="2">
+        <v>250</v>
+      </c>
+      <c r="F48" s="2">
+        <v>250</v>
+      </c>
+      <c r="G48" s="2">
+        <v>125</v>
+      </c>
+      <c r="H48" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>265</v>
       </c>
@@ -3010,8 +5089,23 @@
       <c r="C49" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E49" s="2">
+        <v>250</v>
+      </c>
+      <c r="F49" s="2">
+        <v>250</v>
+      </c>
+      <c r="G49" s="2">
+        <v>250</v>
+      </c>
+      <c r="H49" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>258</v>
       </c>
@@ -3021,8 +5115,23 @@
       <c r="C50" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E50" s="2">
+        <v>250</v>
+      </c>
+      <c r="F50" s="2">
+        <v>250</v>
+      </c>
+      <c r="G50" s="2">
+        <v>125</v>
+      </c>
+      <c r="H50" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>266</v>
       </c>
@@ -3032,8 +5141,23 @@
       <c r="C51" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E51" s="2">
+        <v>250</v>
+      </c>
+      <c r="F51" s="2">
+        <v>250</v>
+      </c>
+      <c r="G51" s="2">
+        <v>250</v>
+      </c>
+      <c r="H51" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>269</v>
       </c>
@@ -3043,8 +5167,23 @@
       <c r="C52" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E52" s="2">
+        <v>250</v>
+      </c>
+      <c r="F52" s="2">
+        <v>250</v>
+      </c>
+      <c r="G52" s="2">
+        <v>125</v>
+      </c>
+      <c r="H52" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>270</v>
       </c>
@@ -3054,8 +5193,23 @@
       <c r="C53" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E53" s="2">
+        <v>250</v>
+      </c>
+      <c r="F53" s="2">
+        <v>250</v>
+      </c>
+      <c r="G53" s="2">
+        <v>250</v>
+      </c>
+      <c r="H53" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>288</v>
       </c>
@@ -3065,8 +5219,23 @@
       <c r="C54" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E54" s="2">
+        <v>250</v>
+      </c>
+      <c r="F54" s="2">
+        <v>250</v>
+      </c>
+      <c r="G54" s="2">
+        <v>125</v>
+      </c>
+      <c r="H54" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>289</v>
       </c>
@@ -3076,8 +5245,23 @@
       <c r="C55" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E55" s="2">
+        <v>250</v>
+      </c>
+      <c r="F55" s="2">
+        <v>250</v>
+      </c>
+      <c r="G55" s="2">
+        <v>250</v>
+      </c>
+      <c r="H55" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>290</v>
       </c>
@@ -3087,8 +5271,23 @@
       <c r="C56" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E56" s="2">
+        <v>250</v>
+      </c>
+      <c r="F56" s="2">
+        <v>250</v>
+      </c>
+      <c r="G56" s="2">
+        <v>125</v>
+      </c>
+      <c r="H56" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>291</v>
       </c>
@@ -3098,8 +5297,23 @@
       <c r="C57" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E57" s="2">
+        <v>250</v>
+      </c>
+      <c r="F57" s="2">
+        <v>250</v>
+      </c>
+      <c r="G57" s="2">
+        <v>250</v>
+      </c>
+      <c r="H57" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>261</v>
       </c>
@@ -3109,8 +5323,23 @@
       <c r="C58" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D58" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E58" s="2">
+        <v>250</v>
+      </c>
+      <c r="F58" s="2">
+        <v>250</v>
+      </c>
+      <c r="G58" s="2">
+        <v>125</v>
+      </c>
+      <c r="H58" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>267</v>
       </c>
@@ -3120,8 +5349,23 @@
       <c r="C59" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D59" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E59" s="2">
+        <v>250</v>
+      </c>
+      <c r="F59" s="2">
+        <v>250</v>
+      </c>
+      <c r="G59" s="2">
+        <v>250</v>
+      </c>
+      <c r="H59" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>262</v>
       </c>
@@ -3131,8 +5375,23 @@
       <c r="C60" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D60" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E60" s="2">
+        <v>250</v>
+      </c>
+      <c r="F60" s="2">
+        <v>250</v>
+      </c>
+      <c r="G60" s="2">
+        <v>125</v>
+      </c>
+      <c r="H60" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>268</v>
       </c>
@@ -3142,8 +5401,23 @@
       <c r="C61" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D61" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E61" s="2">
+        <v>250</v>
+      </c>
+      <c r="F61" s="2">
+        <v>250</v>
+      </c>
+      <c r="G61" s="2">
+        <v>250</v>
+      </c>
+      <c r="H61" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>273</v>
       </c>
@@ -3153,8 +5427,23 @@
       <c r="C62" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D62" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E62" s="2">
+        <v>250</v>
+      </c>
+      <c r="F62" s="2">
+        <v>250</v>
+      </c>
+      <c r="G62" s="2">
+        <v>250</v>
+      </c>
+      <c r="H62" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>274</v>
       </c>
@@ -3164,8 +5453,23 @@
       <c r="C63" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D63" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E63" s="2">
+        <v>250</v>
+      </c>
+      <c r="F63" s="2">
+        <v>250</v>
+      </c>
+      <c r="G63" s="2">
+        <v>250</v>
+      </c>
+      <c r="H63" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>276</v>
       </c>
@@ -3175,8 +5479,23 @@
       <c r="C64" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D64" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E64" s="2">
+        <v>250</v>
+      </c>
+      <c r="F64" s="2">
+        <v>250</v>
+      </c>
+      <c r="G64" s="2">
+        <v>125</v>
+      </c>
+      <c r="H64" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>280</v>
       </c>
@@ -3186,8 +5505,23 @@
       <c r="C65" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D65" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E65" s="2">
+        <v>250</v>
+      </c>
+      <c r="F65" s="2">
+        <v>250</v>
+      </c>
+      <c r="G65" s="2">
+        <v>250</v>
+      </c>
+      <c r="H65" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>282</v>
       </c>
@@ -3197,8 +5531,23 @@
       <c r="C66" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D66" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E66" s="2">
+        <v>250</v>
+      </c>
+      <c r="F66" s="2">
+        <v>250</v>
+      </c>
+      <c r="G66" s="2">
+        <v>250</v>
+      </c>
+      <c r="H66" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>277</v>
       </c>
@@ -3208,8 +5557,23 @@
       <c r="C67" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D67" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E67" s="2">
+        <v>250</v>
+      </c>
+      <c r="F67" s="2">
+        <v>250</v>
+      </c>
+      <c r="G67" s="2">
+        <v>125</v>
+      </c>
+      <c r="H67" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>281</v>
       </c>
@@ -3219,8 +5583,23 @@
       <c r="C68" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D68" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E68" s="2">
+        <v>250</v>
+      </c>
+      <c r="F68" s="2">
+        <v>250</v>
+      </c>
+      <c r="G68" s="2">
+        <v>250</v>
+      </c>
+      <c r="H68" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>283</v>
       </c>
@@ -3230,8 +5609,23 @@
       <c r="C69" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D69" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E69" s="2">
+        <v>250</v>
+      </c>
+      <c r="F69" s="2">
+        <v>250</v>
+      </c>
+      <c r="G69" s="2">
+        <v>250</v>
+      </c>
+      <c r="H69" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>284</v>
       </c>
@@ -3241,8 +5635,23 @@
       <c r="C70" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D70" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E70" s="2">
+        <v>150</v>
+      </c>
+      <c r="F70" s="2">
+        <v>150</v>
+      </c>
+      <c r="G70" s="2">
+        <v>150</v>
+      </c>
+      <c r="H70" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>285</v>
       </c>
@@ -3252,8 +5661,23 @@
       <c r="C71" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D71" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E71" s="2">
+        <v>150</v>
+      </c>
+      <c r="F71" s="2">
+        <v>150</v>
+      </c>
+      <c r="G71" s="2">
+        <v>150</v>
+      </c>
+      <c r="H71" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>286</v>
       </c>
@@ -3263,8 +5687,23 @@
       <c r="C72" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D72" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E72" s="2">
+        <v>150</v>
+      </c>
+      <c r="F72" s="2">
+        <v>150</v>
+      </c>
+      <c r="G72" s="2">
+        <v>150</v>
+      </c>
+      <c r="H72" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>287</v>
       </c>
@@ -3274,8 +5713,23 @@
       <c r="C73" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D73" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E73" s="2">
+        <v>150</v>
+      </c>
+      <c r="F73" s="2">
+        <v>150</v>
+      </c>
+      <c r="G73" s="2">
+        <v>150</v>
+      </c>
+      <c r="H73" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>294</v>
       </c>
@@ -3285,8 +5739,23 @@
       <c r="C74" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D74" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E74" s="2">
+        <v>250</v>
+      </c>
+      <c r="F74" s="2">
+        <v>250</v>
+      </c>
+      <c r="G74" s="2">
+        <v>125</v>
+      </c>
+      <c r="H74" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>297</v>
       </c>
@@ -3296,8 +5765,23 @@
       <c r="C75" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D75" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E75" s="2">
+        <v>250</v>
+      </c>
+      <c r="F75" s="2">
+        <v>250</v>
+      </c>
+      <c r="G75" s="2">
+        <v>125</v>
+      </c>
+      <c r="H75" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>298</v>
       </c>
@@ -3307,8 +5791,23 @@
       <c r="C76" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D76" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E76" s="2">
+        <v>150</v>
+      </c>
+      <c r="F76" s="2">
+        <v>150</v>
+      </c>
+      <c r="G76" s="2">
+        <v>150</v>
+      </c>
+      <c r="H76" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>300</v>
       </c>
@@ -3318,8 +5817,23 @@
       <c r="C77" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D77" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E77" s="2">
+        <v>150</v>
+      </c>
+      <c r="F77" s="2">
+        <v>150</v>
+      </c>
+      <c r="G77" s="2">
+        <v>150</v>
+      </c>
+      <c r="H77" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>306</v>
       </c>
@@ -3329,8 +5843,23 @@
       <c r="C78" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D78" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E78" s="2">
+        <v>150</v>
+      </c>
+      <c r="F78" s="2">
+        <v>150</v>
+      </c>
+      <c r="G78" s="2">
+        <v>150</v>
+      </c>
+      <c r="H78" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>302</v>
       </c>
@@ -3340,8 +5869,23 @@
       <c r="C79" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D79" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E79" s="2">
+        <v>150</v>
+      </c>
+      <c r="F79" s="2">
+        <v>150</v>
+      </c>
+      <c r="G79" s="2">
+        <v>150</v>
+      </c>
+      <c r="H79" s="2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>307</v>
       </c>
@@ -3351,8 +5895,23 @@
       <c r="C80" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D80" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E80" s="2">
+        <v>150</v>
+      </c>
+      <c r="F80" s="2">
+        <v>150</v>
+      </c>
+      <c r="G80" s="2">
+        <v>150</v>
+      </c>
+      <c r="H80" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>303</v>
       </c>
@@ -3362,8 +5921,23 @@
       <c r="C81" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D81" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E81" s="2">
+        <v>150</v>
+      </c>
+      <c r="F81" s="2">
+        <v>150</v>
+      </c>
+      <c r="G81" s="2">
+        <v>150</v>
+      </c>
+      <c r="H81" s="2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>308</v>
       </c>
@@ -3373,8 +5947,23 @@
       <c r="C82" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D82" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E82" s="2">
+        <v>150</v>
+      </c>
+      <c r="F82" s="2">
+        <v>150</v>
+      </c>
+      <c r="G82" s="2">
+        <v>150</v>
+      </c>
+      <c r="H82" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>304</v>
       </c>
@@ -3384,8 +5973,23 @@
       <c r="C83" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D83" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E83" s="2">
+        <v>550</v>
+      </c>
+      <c r="F83" s="2">
+        <v>550</v>
+      </c>
+      <c r="G83" s="2">
+        <v>0</v>
+      </c>
+      <c r="H83" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>309</v>
       </c>
@@ -3395,8 +5999,23 @@
       <c r="C84" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D84" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E84" s="2">
+        <v>550</v>
+      </c>
+      <c r="F84" s="2">
+        <v>550</v>
+      </c>
+      <c r="G84" s="2">
+        <v>0</v>
+      </c>
+      <c r="H84" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>305</v>
       </c>
@@ -3406,8 +6025,23 @@
       <c r="C85" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D85" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E85" s="2">
+        <v>100</v>
+      </c>
+      <c r="F85" s="2">
+        <v>100</v>
+      </c>
+      <c r="G85" s="2">
+        <v>100</v>
+      </c>
+      <c r="H85" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>310</v>
       </c>
@@ -3416,6 +6050,21 @@
       </c>
       <c r="C86" t="s">
         <v>322</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E86" s="2">
+        <v>100</v>
+      </c>
+      <c r="F86" s="2">
+        <v>100</v>
+      </c>
+      <c r="G86" s="2">
+        <v>100</v>
+      </c>
+      <c r="H86" s="2">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -3424,5 +6073,6 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
commit division ucs polygon with columns (#1222)
Co-authored-by: 汤永靖 <tangyongjing@thape.com.cn>
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/连线功能白名单.xlsx
+++ b/AutoLoader/Contents/Support/连线功能白名单.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="火灾报警" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="336">
   <si>
     <t>名称</t>
   </si>
@@ -1177,12 +1177,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1197,11 +1203,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1484,21 +1491,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" customWidth="1"/>
-    <col min="4" max="4" width="21.77734375" customWidth="1"/>
+    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.75" customWidth="1"/>
+    <col min="4" max="4" width="21.75" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
     <col min="6" max="9" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>165</v>
       </c>
@@ -1527,7 +1534,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1553,7 +1560,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1579,7 +1586,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1605,7 +1612,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1631,7 +1638,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1657,7 +1664,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1683,7 +1690,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1709,7 +1716,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1735,7 +1742,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1761,7 +1768,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1787,7 +1794,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1813,7 +1820,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1839,7 +1846,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1865,7 +1872,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1891,7 +1898,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1917,7 +1924,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1943,7 +1950,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1969,7 +1976,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1998,7 +2005,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -2024,7 +2031,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -2050,7 +2057,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -2076,7 +2083,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -2102,7 +2109,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -2128,7 +2135,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -2154,7 +2161,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -2183,7 +2190,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -2209,7 +2216,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -2235,7 +2242,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -2261,7 +2268,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -2287,7 +2294,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>59</v>
       </c>
@@ -2313,7 +2320,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -2339,7 +2346,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -2365,7 +2372,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -2391,7 +2398,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -2417,7 +2424,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -2443,7 +2450,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>71</v>
       </c>
@@ -2469,7 +2476,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>73</v>
       </c>
@@ -2495,7 +2502,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -2521,7 +2528,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -2550,7 +2557,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>79</v>
       </c>
@@ -2576,7 +2583,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>81</v>
       </c>
@@ -2602,7 +2609,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>83</v>
       </c>
@@ -2612,6 +2619,9 @@
       <c r="C43" t="s">
         <v>310</v>
       </c>
+      <c r="D43" t="s">
+        <v>311</v>
+      </c>
       <c r="E43" s="1" t="s">
         <v>331</v>
       </c>
@@ -2628,7 +2638,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>85</v>
       </c>
@@ -2638,6 +2648,9 @@
       <c r="C44" t="s">
         <v>310</v>
       </c>
+      <c r="D44" t="s">
+        <v>311</v>
+      </c>
       <c r="E44" s="1" t="s">
         <v>333</v>
       </c>
@@ -2654,7 +2667,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>87</v>
       </c>
@@ -2664,6 +2677,9 @@
       <c r="C45" t="s">
         <v>310</v>
       </c>
+      <c r="D45" t="s">
+        <v>311</v>
+      </c>
       <c r="E45" s="1" t="s">
         <v>333</v>
       </c>
@@ -2680,7 +2696,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>89</v>
       </c>
@@ -2690,6 +2706,9 @@
       <c r="C46" t="s">
         <v>310</v>
       </c>
+      <c r="D46" t="s">
+        <v>311</v>
+      </c>
       <c r="E46" s="1" t="s">
         <v>333</v>
       </c>
@@ -2706,7 +2725,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>91</v>
       </c>
@@ -2732,7 +2751,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>93</v>
       </c>
@@ -2758,7 +2777,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>94</v>
       </c>
@@ -2784,7 +2803,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>95</v>
       </c>
@@ -2810,7 +2829,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>97</v>
       </c>
@@ -2836,7 +2855,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>99</v>
       </c>
@@ -2865,7 +2884,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>101</v>
       </c>
@@ -2894,7 +2913,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>103</v>
       </c>
@@ -2920,7 +2939,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>105</v>
       </c>
@@ -2946,7 +2965,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>107</v>
       </c>
@@ -2975,7 +2994,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>109</v>
       </c>
@@ -3001,7 +3020,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>111</v>
       </c>
@@ -3027,7 +3046,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>113</v>
       </c>
@@ -3056,7 +3075,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>115</v>
       </c>
@@ -3082,7 +3101,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>117</v>
       </c>
@@ -3108,7 +3127,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>119</v>
       </c>
@@ -3137,7 +3156,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>121</v>
       </c>
@@ -3163,7 +3182,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>123</v>
       </c>
@@ -3192,7 +3211,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>125</v>
       </c>
@@ -3218,7 +3237,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>127</v>
       </c>
@@ -3244,7 +3263,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>129</v>
       </c>
@@ -3270,7 +3289,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>131</v>
       </c>
@@ -3296,7 +3315,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>132</v>
       </c>
@@ -3322,7 +3341,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>133</v>
       </c>
@@ -3348,7 +3367,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>134</v>
       </c>
@@ -3377,7 +3396,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>135</v>
       </c>
@@ -3406,7 +3425,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>136</v>
       </c>
@@ -3435,7 +3454,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>137</v>
       </c>
@@ -3461,7 +3480,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>139</v>
       </c>
@@ -3487,7 +3506,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>141</v>
       </c>
@@ -3513,7 +3532,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>143</v>
       </c>
@@ -3539,7 +3558,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>145</v>
       </c>
@@ -3565,7 +3584,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>147</v>
       </c>
@@ -3591,7 +3610,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>149</v>
       </c>
@@ -3617,7 +3636,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>151</v>
       </c>
@@ -3643,7 +3662,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>153</v>
       </c>
@@ -3669,7 +3688,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>155</v>
       </c>
@@ -3695,7 +3714,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>157</v>
       </c>
@@ -3721,7 +3740,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>159</v>
       </c>
@@ -3747,7 +3766,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>161</v>
       </c>
@@ -3773,7 +3792,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>163</v>
       </c>
@@ -3809,18 +3828,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="33.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.625" customWidth="1"/>
+    <col min="3" max="3" width="33.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>165</v>
       </c>
@@ -3846,7 +3865,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>168</v>
       </c>
@@ -3872,7 +3891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>169</v>
       </c>
@@ -3898,7 +3917,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>170</v>
       </c>
@@ -3924,7 +3943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>171</v>
       </c>
@@ -3950,7 +3969,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>172</v>
       </c>
@@ -3976,7 +3995,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>173</v>
       </c>
@@ -4002,7 +4021,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>174</v>
       </c>
@@ -4028,7 +4047,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>175</v>
       </c>
@@ -4054,7 +4073,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>190</v>
       </c>
@@ -4080,7 +4099,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>185</v>
       </c>
@@ -4106,7 +4125,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>193</v>
       </c>
@@ -4132,7 +4151,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>186</v>
       </c>
@@ -4158,7 +4177,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>194</v>
       </c>
@@ -4184,7 +4203,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>187</v>
       </c>
@@ -4210,7 +4229,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>218</v>
       </c>
@@ -4236,7 +4255,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>219</v>
       </c>
@@ -4262,7 +4281,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>220</v>
       </c>
@@ -4288,7 +4307,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>222</v>
       </c>
@@ -4314,7 +4333,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>221</v>
       </c>
@@ -4340,7 +4359,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>205</v>
       </c>
@@ -4366,7 +4385,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>195</v>
       </c>
@@ -4392,7 +4411,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>196</v>
       </c>
@@ -4418,7 +4437,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>201</v>
       </c>
@@ -4444,7 +4463,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>215</v>
       </c>
@@ -4470,7 +4489,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>199</v>
       </c>
@@ -4496,7 +4515,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>200</v>
       </c>
@@ -4522,7 +4541,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>225</v>
       </c>
@@ -4548,7 +4567,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>210</v>
       </c>
@@ -4574,7 +4593,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>211</v>
       </c>
@@ -4600,7 +4619,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>207</v>
       </c>
@@ -4630,7 +4649,7 @@
         <v>212.13203435596424</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>208</v>
       </c>
@@ -4660,7 +4679,7 @@
         <v>212.13203435596424</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>217</v>
       </c>
@@ -4686,7 +4705,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>235</v>
       </c>
@@ -4712,7 +4731,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>236</v>
       </c>
@@ -4738,7 +4757,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>229</v>
       </c>
@@ -4764,7 +4783,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>230</v>
       </c>
@@ -4790,7 +4809,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>231</v>
       </c>
@@ -4816,7 +4835,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>227</v>
       </c>
@@ -4842,7 +4861,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>239</v>
       </c>
@@ -4868,7 +4887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>240</v>
       </c>
@@ -4894,7 +4913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>243</v>
       </c>
@@ -4920,7 +4939,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>244</v>
       </c>
@@ -4946,7 +4965,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>245</v>
       </c>
@@ -4972,7 +4991,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>246</v>
       </c>
@@ -4998,7 +5017,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>247</v>
       </c>
@@ -5024,7 +5043,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>255</v>
       </c>
@@ -5050,7 +5069,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>263</v>
       </c>
@@ -5076,7 +5095,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>256</v>
       </c>
@@ -5102,7 +5121,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>264</v>
       </c>
@@ -5128,7 +5147,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>267</v>
       </c>
@@ -5154,7 +5173,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>268</v>
       </c>
@@ -5180,7 +5199,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>286</v>
       </c>
@@ -5206,7 +5225,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>287</v>
       </c>
@@ -5232,7 +5251,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>288</v>
       </c>
@@ -5258,7 +5277,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>289</v>
       </c>
@@ -5284,7 +5303,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>259</v>
       </c>
@@ -5310,7 +5329,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>265</v>
       </c>
@@ -5336,7 +5355,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>260</v>
       </c>
@@ -5362,7 +5381,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>266</v>
       </c>
@@ -5388,7 +5407,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>271</v>
       </c>
@@ -5414,7 +5433,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>272</v>
       </c>
@@ -5440,7 +5459,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>274</v>
       </c>
@@ -5466,7 +5485,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>278</v>
       </c>
@@ -5492,7 +5511,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>280</v>
       </c>
@@ -5518,7 +5537,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>275</v>
       </c>
@@ -5544,7 +5563,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>279</v>
       </c>
@@ -5570,7 +5589,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>281</v>
       </c>
@@ -5596,14 +5615,14 @@
         <v>125</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>282</v>
       </c>
       <c r="B69" t="s">
         <v>276</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="2" t="s">
         <v>320</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -5622,14 +5641,14 @@
         <v>150</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>283</v>
       </c>
       <c r="B70" t="s">
         <v>276</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="2" t="s">
         <v>320</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -5648,14 +5667,14 @@
         <v>150</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>284</v>
       </c>
       <c r="B71" t="s">
         <v>276</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="2" t="s">
         <v>320</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -5674,14 +5693,14 @@
         <v>150</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>285</v>
       </c>
       <c r="B72" t="s">
         <v>276</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="2" t="s">
         <v>320</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -5700,7 +5719,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>292</v>
       </c>
@@ -5726,14 +5745,14 @@
         <v>125</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>295</v>
       </c>
       <c r="B74" t="s">
         <v>294</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="2" t="s">
         <v>320</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -5752,7 +5771,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>296</v>
       </c>
@@ -5778,7 +5797,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>298</v>
       </c>
@@ -5804,7 +5823,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>304</v>
       </c>
@@ -5830,7 +5849,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>300</v>
       </c>
@@ -5856,7 +5875,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>305</v>
       </c>
@@ -5882,7 +5901,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>301</v>
       </c>
@@ -5908,7 +5927,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>306</v>
       </c>
@@ -5934,7 +5953,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>302</v>
       </c>
@@ -5960,7 +5979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>307</v>
       </c>
@@ -5986,7 +6005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>303</v>
       </c>
@@ -6012,7 +6031,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>308</v>
       </c>

</xml_diff>

<commit_message>
Update Room configuration and wire connect files
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/连线功能白名单.xlsx
+++ b/AutoLoader/Contents/Support/连线功能白名单.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="火灾报警" sheetId="1" r:id="rId1"/>
@@ -1492,20 +1492,20 @@
   <dimension ref="A1:I87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.75" customWidth="1"/>
-    <col min="4" max="4" width="21.75" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
     <col min="6" max="9" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>165</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1912,19 +1912,19 @@
         <v>333</v>
       </c>
       <c r="F16" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="G16" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="H16" s="1">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="I16" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1938,19 +1938,19 @@
         <v>333</v>
       </c>
       <c r="F17" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="G17" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="H17" s="1">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="I17" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1964,19 +1964,19 @@
         <v>332</v>
       </c>
       <c r="F18" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="G18" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="H18" s="1">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="I18" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -2230,19 +2230,19 @@
         <v>332</v>
       </c>
       <c r="F28" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="G28" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="H28" s="1">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="I28" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>59</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -2412,19 +2412,19 @@
         <v>333</v>
       </c>
       <c r="F35" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="G35" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="H35" s="1">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="I35" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>71</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>73</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>79</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>81</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>83</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>85</v>
       </c>
@@ -2655,19 +2655,19 @@
         <v>333</v>
       </c>
       <c r="F44" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="G44" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="H44" s="1">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="I44" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>87</v>
       </c>
@@ -2684,19 +2684,19 @@
         <v>333</v>
       </c>
       <c r="F45" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="G45" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="H45" s="1">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="I45" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>89</v>
       </c>
@@ -2713,19 +2713,19 @@
         <v>333</v>
       </c>
       <c r="F46" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="G46" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="H46" s="1">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="I46" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>91</v>
       </c>
@@ -2739,19 +2739,19 @@
         <v>332</v>
       </c>
       <c r="F47" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="G47" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="H47" s="1">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="I47" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>93</v>
       </c>
@@ -2765,19 +2765,19 @@
         <v>333</v>
       </c>
       <c r="F48" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="G48" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="H48" s="1">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="I48" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>94</v>
       </c>
@@ -2791,19 +2791,19 @@
         <v>333</v>
       </c>
       <c r="F49" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="G49" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="H49" s="1">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="I49" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>95</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>97</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>99</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>101</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>103</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>105</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>107</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>109</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>111</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>113</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>115</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>117</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>119</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>121</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>123</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>125</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>127</v>
       </c>
@@ -3257,7 +3257,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>129</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>131</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>132</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>133</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>134</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>135</v>
       </c>
@@ -3419,7 +3419,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>136</v>
       </c>
@@ -3448,7 +3448,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>137</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>139</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>141</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>143</v>
       </c>
@@ -3552,7 +3552,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>145</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>147</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>149</v>
       </c>
@@ -3630,7 +3630,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>151</v>
       </c>
@@ -3656,7 +3656,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>153</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>155</v>
       </c>
@@ -3708,7 +3708,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>157</v>
       </c>
@@ -3734,7 +3734,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>159</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>161</v>
       </c>
@@ -3786,7 +3786,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>163</v>
       </c>
@@ -3815,6 +3815,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3826,14 +3827,14 @@
       <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.625" customWidth="1"/>
-    <col min="3" max="3" width="33.875" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="33.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>165</v>
       </c>
@@ -3859,7 +3860,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>168</v>
       </c>
@@ -3885,7 +3886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>169</v>
       </c>
@@ -3911,7 +3912,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>170</v>
       </c>
@@ -3937,7 +3938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>171</v>
       </c>
@@ -3963,7 +3964,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>172</v>
       </c>
@@ -3989,7 +3990,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>173</v>
       </c>
@@ -4015,7 +4016,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>174</v>
       </c>
@@ -4041,7 +4042,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>175</v>
       </c>
@@ -4067,7 +4068,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>190</v>
       </c>
@@ -4093,7 +4094,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>185</v>
       </c>
@@ -4119,7 +4120,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>193</v>
       </c>
@@ -4145,7 +4146,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>186</v>
       </c>
@@ -4171,7 +4172,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>194</v>
       </c>
@@ -4197,7 +4198,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>187</v>
       </c>
@@ -4223,7 +4224,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>218</v>
       </c>
@@ -4249,7 +4250,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>219</v>
       </c>
@@ -4275,7 +4276,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>220</v>
       </c>
@@ -4301,7 +4302,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>222</v>
       </c>
@@ -4327,7 +4328,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>221</v>
       </c>
@@ -4353,7 +4354,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>205</v>
       </c>
@@ -4379,7 +4380,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>195</v>
       </c>
@@ -4405,7 +4406,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>196</v>
       </c>
@@ -4431,7 +4432,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>201</v>
       </c>
@@ -4457,7 +4458,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>215</v>
       </c>
@@ -4483,7 +4484,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>199</v>
       </c>
@@ -4509,7 +4510,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>200</v>
       </c>
@@ -4535,7 +4536,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>225</v>
       </c>
@@ -4561,7 +4562,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>210</v>
       </c>
@@ -4587,7 +4588,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>211</v>
       </c>
@@ -4613,7 +4614,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>207</v>
       </c>
@@ -4643,7 +4644,7 @@
         <v>212.13203435596424</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>208</v>
       </c>
@@ -4673,7 +4674,7 @@
         <v>212.13203435596424</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>217</v>
       </c>
@@ -4699,7 +4700,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>235</v>
       </c>
@@ -4725,7 +4726,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>236</v>
       </c>
@@ -4751,7 +4752,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>229</v>
       </c>
@@ -4777,7 +4778,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>230</v>
       </c>
@@ -4803,7 +4804,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>231</v>
       </c>
@@ -4829,7 +4830,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>227</v>
       </c>
@@ -4855,7 +4856,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>239</v>
       </c>
@@ -4881,7 +4882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>240</v>
       </c>
@@ -4907,7 +4908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>243</v>
       </c>
@@ -4933,7 +4934,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>244</v>
       </c>
@@ -4959,7 +4960,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>245</v>
       </c>
@@ -4985,7 +4986,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>246</v>
       </c>
@@ -5011,7 +5012,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>247</v>
       </c>
@@ -5037,7 +5038,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>255</v>
       </c>
@@ -5063,7 +5064,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>263</v>
       </c>
@@ -5089,7 +5090,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>256</v>
       </c>
@@ -5115,7 +5116,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>264</v>
       </c>
@@ -5141,7 +5142,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>267</v>
       </c>
@@ -5167,7 +5168,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>268</v>
       </c>
@@ -5193,7 +5194,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>286</v>
       </c>
@@ -5219,7 +5220,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>287</v>
       </c>
@@ -5245,7 +5246,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>288</v>
       </c>
@@ -5271,7 +5272,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>289</v>
       </c>
@@ -5297,7 +5298,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>259</v>
       </c>
@@ -5323,7 +5324,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>265</v>
       </c>
@@ -5349,7 +5350,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>260</v>
       </c>
@@ -5375,7 +5376,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>266</v>
       </c>
@@ -5401,7 +5402,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>271</v>
       </c>
@@ -5427,7 +5428,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>272</v>
       </c>
@@ -5453,7 +5454,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>274</v>
       </c>
@@ -5479,7 +5480,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>278</v>
       </c>
@@ -5505,7 +5506,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>280</v>
       </c>
@@ -5531,7 +5532,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>275</v>
       </c>
@@ -5557,7 +5558,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>279</v>
       </c>
@@ -5583,7 +5584,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>281</v>
       </c>
@@ -5609,7 +5610,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>282</v>
       </c>
@@ -5635,7 +5636,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>283</v>
       </c>
@@ -5661,7 +5662,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>284</v>
       </c>
@@ -5687,7 +5688,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>285</v>
       </c>
@@ -5713,7 +5714,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>292</v>
       </c>
@@ -5739,7 +5740,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>295</v>
       </c>
@@ -5765,7 +5766,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>296</v>
       </c>
@@ -5791,7 +5792,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>298</v>
       </c>
@@ -5817,7 +5818,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>304</v>
       </c>
@@ -5843,7 +5844,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>300</v>
       </c>
@@ -5869,7 +5870,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>305</v>
       </c>
@@ -5895,7 +5896,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>301</v>
       </c>
@@ -5921,7 +5922,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>306</v>
       </c>
@@ -5947,7 +5948,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>302</v>
       </c>
@@ -5973,7 +5974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>307</v>
       </c>
@@ -5999,7 +6000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>303</v>
       </c>
@@ -6025,7 +6026,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>308</v>
       </c>

</xml_diff>

<commit_message>
commit fix bugs (#2383)
Co-authored-by: 汤永靖 <tangyongjing@thape.com.cn>
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/连线功能白名单.xlsx
+++ b/AutoLoader/Contents/Support/连线功能白名单.xlsx
@@ -1,26 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{127B789D-9359-4755-AF76-27827EBBC086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="14388" yWindow="0" windowWidth="16308" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="火灾报警" sheetId="1" r:id="rId1"/>
     <sheet name="照明" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="341">
   <si>
     <t>名称</t>
   </si>
@@ -1148,13 +1157,41 @@
   </si>
   <si>
     <t>Circle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Install Method</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Density</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL221</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL223</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1197,12 +1234,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1482,24 +1522,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I86"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:XFD42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.75" customWidth="1"/>
-    <col min="4" max="4" width="21.75" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="9" width="9" style="1"/>
+    <col min="6" max="9" width="8.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>163</v>
       </c>
@@ -1527,8 +1569,14 @@
       <c r="I1" s="1" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1553,8 +1601,14 @@
       <c r="I2" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1579,8 +1633,14 @@
       <c r="I3" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1605,8 +1665,14 @@
       <c r="I4" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1631,8 +1697,14 @@
       <c r="I5" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1657,8 +1729,14 @@
       <c r="I6" s="1">
         <v>300</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1683,8 +1761,14 @@
       <c r="I7" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1709,8 +1793,14 @@
       <c r="I8" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1735,8 +1825,14 @@
       <c r="I9" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1761,8 +1857,14 @@
       <c r="I10" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1787,8 +1889,14 @@
       <c r="I11" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1813,8 +1921,14 @@
       <c r="I12" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1839,8 +1953,14 @@
       <c r="I13" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1865,8 +1985,14 @@
       <c r="I14" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1891,8 +2017,14 @@
       <c r="I15" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1917,8 +2049,14 @@
       <c r="I16" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1943,8 +2081,14 @@
       <c r="I17" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1969,8 +2113,14 @@
       <c r="I18" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1998,8 +2148,14 @@
       <c r="I19" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K19" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -2024,8 +2180,14 @@
       <c r="I20" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -2050,8 +2212,14 @@
       <c r="I21" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -2076,8 +2244,14 @@
       <c r="I22" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -2102,8 +2276,14 @@
       <c r="I23" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -2128,8 +2308,14 @@
       <c r="I24" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K24" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -2154,8 +2340,14 @@
       <c r="I25" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J25" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K25" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -2183,8 +2375,14 @@
       <c r="I26" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J26" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K26" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -2209,8 +2407,14 @@
       <c r="I27" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J27" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K27" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -2235,8 +2439,14 @@
       <c r="I28" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J28" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K28" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -2261,8 +2471,14 @@
       <c r="I29" s="1">
         <v>300</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J29" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K29" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -2287,8 +2503,14 @@
       <c r="I30" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J30" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K30" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>59</v>
       </c>
@@ -2313,8 +2535,14 @@
       <c r="I31" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J31" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K31" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -2339,8 +2567,14 @@
       <c r="I32" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J32" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K32" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -2365,8 +2599,14 @@
       <c r="I33" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J33" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K33" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -2391,8 +2631,14 @@
       <c r="I34" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J34" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K34" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -2417,8 +2663,14 @@
       <c r="I35" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J35" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K35" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -2443,8 +2695,14 @@
       <c r="I36" s="1">
         <v>300</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J36" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K36" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>71</v>
       </c>
@@ -2469,8 +2727,14 @@
       <c r="I37" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J37" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K37" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>73</v>
       </c>
@@ -2495,8 +2759,14 @@
       <c r="I38" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J38" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K38" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -2521,8 +2791,14 @@
       <c r="I39" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J39" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K39" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -2550,8 +2826,14 @@
       <c r="I40" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J40" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K40" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>79</v>
       </c>
@@ -2576,8 +2858,14 @@
       <c r="I41" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J41" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K41" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>81</v>
       </c>
@@ -2605,8 +2893,14 @@
       <c r="I42" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J42" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K42" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>83</v>
       </c>
@@ -2634,8 +2928,14 @@
       <c r="I43" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J43" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K43" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>85</v>
       </c>
@@ -2663,8 +2963,14 @@
       <c r="I44" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J44" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K44" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>87</v>
       </c>
@@ -2692,8 +2998,14 @@
       <c r="I45" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J45" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K45" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>89</v>
       </c>
@@ -2718,8 +3030,14 @@
       <c r="I46" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J46" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K46" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>91</v>
       </c>
@@ -2744,8 +3062,14 @@
       <c r="I47" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J47" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K47" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>92</v>
       </c>
@@ -2770,8 +3094,14 @@
       <c r="I48" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J48" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K48" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>93</v>
       </c>
@@ -2796,8 +3126,14 @@
       <c r="I49" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J49" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K49" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>95</v>
       </c>
@@ -2822,8 +3158,14 @@
       <c r="I50" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J50" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K50" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>97</v>
       </c>
@@ -2851,8 +3193,14 @@
       <c r="I51" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J51" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K51" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>99</v>
       </c>
@@ -2880,8 +3228,14 @@
       <c r="I52" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J52" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K52" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>101</v>
       </c>
@@ -2906,8 +3260,14 @@
       <c r="I53" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J53" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K53" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>103</v>
       </c>
@@ -2932,8 +3292,14 @@
       <c r="I54" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J54" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K54" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>105</v>
       </c>
@@ -2961,8 +3327,14 @@
       <c r="I55" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J55" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K55" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>107</v>
       </c>
@@ -2987,8 +3359,14 @@
       <c r="I56" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J56" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K56" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>109</v>
       </c>
@@ -3013,8 +3391,14 @@
       <c r="I57" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J57" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K57" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>111</v>
       </c>
@@ -3039,8 +3423,14 @@
       <c r="I58" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J58" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K58" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>113</v>
       </c>
@@ -3065,8 +3455,14 @@
       <c r="I59" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J59" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K59" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>115</v>
       </c>
@@ -3091,8 +3487,14 @@
       <c r="I60" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J60" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K60" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>117</v>
       </c>
@@ -3120,8 +3522,14 @@
       <c r="I61" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J61" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K61" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>119</v>
       </c>
@@ -3146,8 +3554,14 @@
       <c r="I62" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J62" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K62" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>121</v>
       </c>
@@ -3172,8 +3586,14 @@
       <c r="I63" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J63" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K63" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>123</v>
       </c>
@@ -3198,8 +3618,14 @@
       <c r="I64" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J64" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K64" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>125</v>
       </c>
@@ -3224,8 +3650,14 @@
       <c r="I65" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J65" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K65" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>127</v>
       </c>
@@ -3250,8 +3682,14 @@
       <c r="I66" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J66" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K66" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>129</v>
       </c>
@@ -3276,8 +3714,14 @@
       <c r="I67" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J67" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K67" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>130</v>
       </c>
@@ -3302,8 +3746,14 @@
       <c r="I68" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J68" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K68" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>131</v>
       </c>
@@ -3328,8 +3778,14 @@
       <c r="I69" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J69" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K69" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>132</v>
       </c>
@@ -3357,8 +3813,14 @@
       <c r="I70" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J70" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K70" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>133</v>
       </c>
@@ -3386,8 +3848,14 @@
       <c r="I71" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J71" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K71" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>134</v>
       </c>
@@ -3415,8 +3883,14 @@
       <c r="I72" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J72" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K72" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>135</v>
       </c>
@@ -3441,8 +3915,14 @@
       <c r="I73" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J73" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K73" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>137</v>
       </c>
@@ -3467,8 +3947,14 @@
       <c r="I74" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J74" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K74" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>139</v>
       </c>
@@ -3493,8 +3979,14 @@
       <c r="I75" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J75" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K75" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>141</v>
       </c>
@@ -3519,8 +4011,14 @@
       <c r="I76" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J76" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K76" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>143</v>
       </c>
@@ -3545,8 +4043,14 @@
       <c r="I77" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J77" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K77" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>145</v>
       </c>
@@ -3571,8 +4075,14 @@
       <c r="I78" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J78" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K78" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>147</v>
       </c>
@@ -3597,8 +4107,14 @@
       <c r="I79" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J79" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K79" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>149</v>
       </c>
@@ -3623,8 +4139,14 @@
       <c r="I80" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J80" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="K80" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>151</v>
       </c>
@@ -3649,8 +4171,14 @@
       <c r="I81" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J81" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K81" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>153</v>
       </c>
@@ -3675,8 +4203,14 @@
       <c r="I82" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J82" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K82" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>155</v>
       </c>
@@ -3701,8 +4235,14 @@
       <c r="I83" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J83" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K83" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>157</v>
       </c>
@@ -3727,8 +4267,14 @@
       <c r="I84" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J84" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K84" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>159</v>
       </c>
@@ -3753,8 +4299,14 @@
       <c r="I85" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J85" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K85" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>161</v>
       </c>
@@ -3778,6 +4330,12 @@
       </c>
       <c r="I86" s="1">
         <v>150</v>
+      </c>
+      <c r="J86" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="K86" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3788,21 +4346,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H85"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.625" customWidth="1"/>
-    <col min="3" max="3" width="33.875" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="33.88671875" customWidth="1"/>
+    <col min="4" max="8" width="8.88671875" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>163</v>
       </c>
@@ -3827,8 +4387,14 @@
       <c r="H1" s="1" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>166</v>
       </c>
@@ -3853,8 +4419,14 @@
       <c r="H2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>167</v>
       </c>
@@ -3879,8 +4451,14 @@
       <c r="H3" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>168</v>
       </c>
@@ -3905,8 +4483,14 @@
       <c r="H4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>169</v>
       </c>
@@ -3931,8 +4515,14 @@
       <c r="H5" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>170</v>
       </c>
@@ -3957,8 +4547,14 @@
       <c r="H6" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>171</v>
       </c>
@@ -3983,8 +4579,14 @@
       <c r="H7" s="1">
         <v>300</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>172</v>
       </c>
@@ -4009,8 +4611,14 @@
       <c r="H8" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>173</v>
       </c>
@@ -4035,8 +4643,14 @@
       <c r="H9" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>188</v>
       </c>
@@ -4061,8 +4675,14 @@
       <c r="H10" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>183</v>
       </c>
@@ -4087,8 +4707,14 @@
       <c r="H11" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>191</v>
       </c>
@@ -4113,8 +4739,14 @@
       <c r="H12" s="1">
         <v>300</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J12" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>184</v>
       </c>
@@ -4139,8 +4771,14 @@
       <c r="H13" s="1">
         <v>300</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J13" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>192</v>
       </c>
@@ -4165,8 +4803,14 @@
       <c r="H14" s="1">
         <v>300</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J14" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>185</v>
       </c>
@@ -4191,8 +4835,14 @@
       <c r="H15" s="1">
         <v>300</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J15" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>216</v>
       </c>
@@ -4217,8 +4867,14 @@
       <c r="H16" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>217</v>
       </c>
@@ -4243,8 +4899,14 @@
       <c r="H17" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>218</v>
       </c>
@@ -4269,8 +4931,14 @@
       <c r="H18" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>220</v>
       </c>
@@ -4295,8 +4963,14 @@
       <c r="H19" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>219</v>
       </c>
@@ -4321,8 +4995,14 @@
       <c r="H20" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>203</v>
       </c>
@@ -4347,8 +5027,14 @@
       <c r="H21" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>193</v>
       </c>
@@ -4373,8 +5059,14 @@
       <c r="H22" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>194</v>
       </c>
@@ -4399,8 +5091,14 @@
       <c r="H23" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>199</v>
       </c>
@@ -4425,8 +5123,14 @@
       <c r="H24" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>213</v>
       </c>
@@ -4451,8 +5155,14 @@
       <c r="H25" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>197</v>
       </c>
@@ -4477,8 +5187,14 @@
       <c r="H26" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>198</v>
       </c>
@@ -4503,8 +5219,14 @@
       <c r="H27" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>223</v>
       </c>
@@ -4529,8 +5251,14 @@
       <c r="H28" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>208</v>
       </c>
@@ -4555,8 +5283,14 @@
       <c r="H29" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>209</v>
       </c>
@@ -4581,8 +5315,14 @@
       <c r="H30" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>205</v>
       </c>
@@ -4611,8 +5351,14 @@
         <f t="shared" si="0"/>
         <v>212.13203435596424</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>206</v>
       </c>
@@ -4641,8 +5387,14 @@
         <f t="shared" si="0"/>
         <v>212.13203435596424</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I32" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>215</v>
       </c>
@@ -4667,8 +5419,14 @@
       <c r="H33" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I33" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>233</v>
       </c>
@@ -4693,8 +5451,14 @@
       <c r="H34" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I34" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>234</v>
       </c>
@@ -4719,8 +5483,14 @@
       <c r="H35" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I35" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>227</v>
       </c>
@@ -4745,8 +5515,14 @@
       <c r="H36" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I36" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J36" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>228</v>
       </c>
@@ -4771,8 +5547,14 @@
       <c r="H37" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I37" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>229</v>
       </c>
@@ -4797,8 +5579,14 @@
       <c r="H38" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I38" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>225</v>
       </c>
@@ -4823,8 +5611,14 @@
       <c r="H39" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I39" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="J39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>237</v>
       </c>
@@ -4849,8 +5643,14 @@
       <c r="H40" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I40" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>238</v>
       </c>
@@ -4875,8 +5675,14 @@
       <c r="H41" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I41" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>241</v>
       </c>
@@ -4901,8 +5707,14 @@
       <c r="H42" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I42" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>242</v>
       </c>
@@ -4927,8 +5739,14 @@
       <c r="H43" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I43" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J43" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>243</v>
       </c>
@@ -4953,8 +5771,14 @@
       <c r="H44" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I44" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>244</v>
       </c>
@@ -4979,8 +5803,14 @@
       <c r="H45" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I45" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="J45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>245</v>
       </c>
@@ -5005,8 +5835,14 @@
       <c r="H46" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I46" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>253</v>
       </c>
@@ -5031,8 +5867,14 @@
       <c r="H47" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I47" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J47" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>261</v>
       </c>
@@ -5057,8 +5899,14 @@
       <c r="H48" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I48" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>254</v>
       </c>
@@ -5083,8 +5931,14 @@
       <c r="H49" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I49" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J49" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>262</v>
       </c>
@@ -5109,8 +5963,14 @@
       <c r="H50" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I50" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J50" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>265</v>
       </c>
@@ -5135,8 +5995,14 @@
       <c r="H51" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I51" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J51" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>266</v>
       </c>
@@ -5161,8 +6027,14 @@
       <c r="H52" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I52" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J52" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>284</v>
       </c>
@@ -5187,8 +6059,14 @@
       <c r="H53" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I53" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J53" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>285</v>
       </c>
@@ -5213,8 +6091,14 @@
       <c r="H54" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I54" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>286</v>
       </c>
@@ -5239,8 +6123,14 @@
       <c r="H55" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I55" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>287</v>
       </c>
@@ -5265,8 +6155,14 @@
       <c r="H56" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I56" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J56" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>257</v>
       </c>
@@ -5291,8 +6187,14 @@
       <c r="H57" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I57" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J57" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>263</v>
       </c>
@@ -5317,8 +6219,14 @@
       <c r="H58" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I58" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J58" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>258</v>
       </c>
@@ -5343,8 +6251,14 @@
       <c r="H59" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I59" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>264</v>
       </c>
@@ -5369,8 +6283,14 @@
       <c r="H60" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I60" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J60" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>269</v>
       </c>
@@ -5395,8 +6315,14 @@
       <c r="H61" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I61" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J61" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>270</v>
       </c>
@@ -5421,8 +6347,14 @@
       <c r="H62" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I62" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>272</v>
       </c>
@@ -5447,8 +6379,14 @@
       <c r="H63" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I63" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J63" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>276</v>
       </c>
@@ -5473,8 +6411,14 @@
       <c r="H64" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I64" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>278</v>
       </c>
@@ -5499,8 +6443,14 @@
       <c r="H65" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I65" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J65" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>273</v>
       </c>
@@ -5525,8 +6475,14 @@
       <c r="H66" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I66" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J66" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>277</v>
       </c>
@@ -5551,8 +6507,14 @@
       <c r="H67" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I67" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J67" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>279</v>
       </c>
@@ -5577,10 +6539,16 @@
       <c r="H68" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I68" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J68" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>280</v>
+        <v>339</v>
       </c>
       <c r="B69" t="s">
         <v>274</v>
@@ -5603,10 +6571,16 @@
       <c r="H69" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I69" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J69" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>281</v>
+        <v>340</v>
       </c>
       <c r="B70" t="s">
         <v>274</v>
@@ -5629,10 +6603,16 @@
       <c r="H70" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I70" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="J70" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B71" t="s">
         <v>274</v>
@@ -5641,7 +6621,7 @@
         <v>318</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E71" s="1">
         <v>150</v>
@@ -5655,10 +6635,16 @@
       <c r="H71" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I71" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="J71" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B72" t="s">
         <v>274</v>
@@ -5667,137 +6653,167 @@
         <v>318</v>
       </c>
       <c r="D72" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E72" s="1">
+        <v>150</v>
+      </c>
+      <c r="F72" s="1">
+        <v>150</v>
+      </c>
+      <c r="G72" s="1">
+        <v>150</v>
+      </c>
+      <c r="H72" s="1">
+        <v>150</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="J72" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>282</v>
+      </c>
+      <c r="B73" t="s">
+        <v>274</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="E72" s="1">
-        <v>150</v>
-      </c>
-      <c r="F72" s="1">
-        <v>150</v>
-      </c>
-      <c r="G72" s="1">
-        <v>150</v>
-      </c>
-      <c r="H72" s="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>290</v>
-      </c>
-      <c r="B73" t="s">
-        <v>291</v>
-      </c>
-      <c r="C73" t="s">
-        <v>318</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>325</v>
-      </c>
       <c r="E73" s="1">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="F73" s="1">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="G73" s="1">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="H73" s="1">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="J73" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="B74" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>318</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="E74" s="1">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="F74" s="1">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="G74" s="1">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="H74" s="1">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="J74" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B75" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C75" t="s">
         <v>318</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E75" s="1">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="F75" s="1">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="G75" s="1">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="H75" s="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J75" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B76" t="s">
-        <v>297</v>
-      </c>
-      <c r="C76" t="s">
+        <v>292</v>
+      </c>
+      <c r="C76" s="2" t="s">
         <v>318</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E76" s="1">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="F76" s="1">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="G76" s="1">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="H76" s="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="J76" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="B77" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="C77" t="s">
         <v>318</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E77" s="1">
         <v>150</v>
@@ -5811,19 +6827,25 @@
       <c r="H77" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I77" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="J77" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B78" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="C78" t="s">
         <v>318</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="E78" s="1">
         <v>150</v>
@@ -5835,12 +6857,18 @@
         <v>150</v>
       </c>
       <c r="H78" s="1">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J78" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B79" t="s">
         <v>307</v>
@@ -5863,10 +6891,16 @@
       <c r="H79" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I79" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J79" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B80" t="s">
         <v>307</v>
@@ -5889,10 +6923,16 @@
       <c r="H80" s="1">
         <v>225</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I80" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J80" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B81" t="s">
         <v>307</v>
@@ -5901,7 +6941,7 @@
         <v>318</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="E81" s="1">
         <v>150</v>
@@ -5915,10 +6955,16 @@
       <c r="H81" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I81" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J81" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B82" t="s">
         <v>307</v>
@@ -5930,21 +6976,27 @@
         <v>325</v>
       </c>
       <c r="E82" s="1">
-        <v>550</v>
+        <v>150</v>
       </c>
       <c r="F82" s="1">
-        <v>550</v>
+        <v>150</v>
       </c>
       <c r="G82" s="1">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="H82" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J82" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B83" t="s">
         <v>307</v>
@@ -5953,24 +7005,30 @@
         <v>318</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="E83" s="1">
-        <v>550</v>
+        <v>150</v>
       </c>
       <c r="F83" s="1">
-        <v>550</v>
+        <v>150</v>
       </c>
       <c r="G83" s="1">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="H83" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J83" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B84" t="s">
         <v>307</v>
@@ -5979,24 +7037,30 @@
         <v>318</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E84" s="1">
-        <v>100</v>
+        <v>550</v>
       </c>
       <c r="F84" s="1">
-        <v>100</v>
+        <v>550</v>
       </c>
       <c r="G84" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H84" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J84" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B85" t="s">
         <v>307</v>
@@ -6005,19 +7069,89 @@
         <v>318</v>
       </c>
       <c r="D85" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E85" s="1">
+        <v>550</v>
+      </c>
+      <c r="F85" s="1">
+        <v>550</v>
+      </c>
+      <c r="G85" s="1">
+        <v>0</v>
+      </c>
+      <c r="H85" s="1">
+        <v>0</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J85" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>301</v>
+      </c>
+      <c r="B86" t="s">
+        <v>307</v>
+      </c>
+      <c r="C86" t="s">
+        <v>318</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="E85" s="1">
+      <c r="E86" s="1">
         <v>100</v>
       </c>
-      <c r="F85" s="1">
+      <c r="F86" s="1">
         <v>100</v>
       </c>
-      <c r="G85" s="1">
+      <c r="G86" s="1">
         <v>100</v>
       </c>
-      <c r="H85" s="1">
+      <c r="H86" s="1">
         <v>100</v>
+      </c>
+      <c r="I86" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J86" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>306</v>
+      </c>
+      <c r="B87" t="s">
+        <v>307</v>
+      </c>
+      <c r="C87" t="s">
+        <v>318</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E87" s="1">
+        <v>100</v>
+      </c>
+      <c r="F87" s="1">
+        <v>100</v>
+      </c>
+      <c r="G87" s="1">
+        <v>100</v>
+      </c>
+      <c r="H87" s="1">
+        <v>100</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J87" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>